<commit_message>
Modificado Pom.xml para que copie dependencias
Fuente:
https://es.stackoverflow.com/questions/350588/c%c3%b3mo-funciona-classpath
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="304">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -972,16 +972,22 @@
   <si>
     <t>&lt;/build&gt;</t>
   </si>
+  <si>
+    <t>Copia de Librerias:</t>
+  </si>
+  <si>
+    <t>https://es.stackoverflow.com/questions/350588/c%c3%b3mo-funciona-classpath</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1038,8 +1044,29 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1054,35 +1081,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1096,15 +1095,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1119,40 +1164,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1164,23 +1178,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1261,7 +1267,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,19 +1387,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1297,37 +1423,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1339,97 +1435,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1495,11 +1501,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1519,36 +1531,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1556,15 +1538,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1583,141 +1556,174 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4638,13 +4644,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -4739,6 +4745,16 @@
     <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
listar productos y dump de base de datos
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="9555" tabRatio="916" activeTab="5"/>
+    <workbookView windowWidth="23895" windowHeight="9555" tabRatio="916" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NECESIDADES" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="lista de productos ejemplo" sheetId="3" r:id="rId3"/>
     <sheet name="mysql" sheetId="5" r:id="rId4"/>
     <sheet name="enlaces y recursos JAVA" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="LIBRERIAS Y POM ORG PROY" sheetId="6" r:id="rId6"/>
+    <sheet name="ICONOS" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="326">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -910,6 +911,39 @@
     <t>https://www.youtube.com/watch?v=kPCbb80_6GI</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=Soe5FrO-tp4</t>
+  </si>
+  <si>
+    <t>Como hacer CRUD en Java Escritorio MVC - Listar</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=d7-PPSKgouA</t>
+  </si>
+  <si>
+    <t>Como hacer CRUD en Java Escritorio MVC - Eliminar</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Zg0SMBhZ58s</t>
+  </si>
+  <si>
+    <t>Como hacer CRUD en Java Escritorio MVC - Actualizar</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=30rPFrwMOQI</t>
+  </si>
+  <si>
+    <t>Como hacer CRUD en Java Escritorio MVC - Agregar</t>
+  </si>
+  <si>
+    <t>MYSQL CRUD EN JAVA CON MYSEL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Erw8W5pH_T4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Fxk77AJPejM</t>
+  </si>
+  <si>
     <t>UN M MONTON DE EJEMPLOS</t>
   </si>
   <si>
@@ -977,6 +1011,39 @@
   </si>
   <si>
     <t>https://es.stackoverflow.com/questions/350588/c%c3%b3mo-funciona-classpath</t>
+  </si>
+  <si>
+    <t>https://wwwhatsnew.com/2017/01/19/10-buscadores-para-bajar-iconos-gratis/</t>
+  </si>
+  <si>
+    <t>https://www.flaticon.es/</t>
+  </si>
+  <si>
+    <t>https://icons8.com/icons/new</t>
+  </si>
+  <si>
+    <t>https://mricons.com/</t>
+  </si>
+  <si>
+    <t>https://www.iconspedia.com/</t>
+  </si>
+  <si>
+    <t>https://www.iconseeker.com/</t>
+  </si>
+  <si>
+    <t>https://www.iconfinder.com/</t>
+  </si>
+  <si>
+    <t>https://iconarchive.com/</t>
+  </si>
+  <si>
+    <t>https://roundicons.com/</t>
+  </si>
+  <si>
+    <t>https://video-editor.online/</t>
+  </si>
+  <si>
+    <t>https://tablericons.com/</t>
   </si>
 </sst>
 </file>
@@ -985,11 +1052,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1012,6 +1079,12 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Roboto"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1044,9 +1117,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1058,7 +1131,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1066,14 +1139,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1087,24 +1176,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1118,22 +1191,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1149,18 +1216,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1171,22 +1244,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1273,7 +1346,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1285,13 +1370,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1303,7 +1406,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,91 +1472,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1411,31 +1502,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1501,6 +1574,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1512,6 +1618,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1531,17 +1648,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1556,178 +1662,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1740,51 +1813,52 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1807,19 +1881,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2488,20 +2562,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="3:11">
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
       <c r="K3" t="s">
         <v>20</v>
       </c>
@@ -2517,87 +2591,87 @@
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="26" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="35" t="s">
         <v>29</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" ht="21" spans="3:8">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="29" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="4:8">
-      <c r="D9" s="29">
+      <c r="D9" s="30">
         <v>45</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="30">
         <v>150</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="3:3">
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="3:9">
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="32" t="s">
         <v>37</v>
       </c>
       <c r="I13" t="s">
@@ -2605,19 +2679,19 @@
       </c>
     </row>
     <row r="14" spans="3:9">
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="33" t="s">
         <v>40</v>
       </c>
       <c r="I14" t="s">
@@ -2630,65 +2704,65 @@
       </c>
     </row>
     <row r="20" spans="3:3">
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="26" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="3:11">
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="K21" s="37" t="s">
+      <c r="K21" s="38" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="3:11">
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="30" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2707,7 +2781,7 @@
   <sheetPr/>
   <dimension ref="B2:C210"/>
   <sheetViews>
-    <sheetView topLeftCell="A181" workbookViewId="0">
+    <sheetView topLeftCell="A154" workbookViewId="0">
       <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
@@ -2719,1636 +2793,1636 @@
   <sheetData>
     <row r="2" ht="13.5"/>
     <row r="3" ht="13.5" spans="2:3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" ht="13.5" spans="2:3">
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" ht="13.5" spans="2:3">
-      <c r="B5" s="10">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" ht="13.5" spans="2:3">
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" ht="13.5" spans="2:3">
-      <c r="B7" s="10">
+      <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" ht="13.5" spans="2:3">
-      <c r="B8" s="10">
+      <c r="B8" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" ht="13.5" spans="2:3">
-      <c r="B9" s="10">
+      <c r="B9" s="11">
         <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" ht="13.5" spans="2:3">
-      <c r="B10" s="10">
+      <c r="B10" s="11">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" ht="13.5" spans="2:3">
-      <c r="B11" s="10">
+      <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" ht="13.5" spans="2:3">
-      <c r="B12" s="10">
+      <c r="B12" s="11">
         <v>9</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" ht="13.5" spans="2:3">
-      <c r="B13" s="10">
+      <c r="B13" s="11">
         <v>10</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" ht="13.5" spans="2:3">
-      <c r="B14" s="10">
+      <c r="B14" s="11">
         <v>11</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" ht="13.5" spans="2:3">
-      <c r="B15" s="10">
+      <c r="B15" s="11">
         <v>12</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" ht="13.5" spans="2:3">
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>13</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" ht="13.5" spans="2:3">
-      <c r="B17" s="10">
+      <c r="B17" s="11">
         <v>14</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" ht="13.5" spans="2:3">
-      <c r="B18" s="10">
+      <c r="B18" s="11">
         <v>15</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" ht="13.5" spans="2:3">
-      <c r="B19" s="10">
+      <c r="B19" s="11">
         <v>16</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="20" ht="13.5" spans="2:3">
-      <c r="B20" s="10">
+      <c r="B20" s="11">
         <v>17</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" ht="13.5" spans="2:3">
-      <c r="B21" s="10">
+      <c r="B21" s="11">
         <v>18</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22" ht="13.5" spans="2:3">
-      <c r="B22" s="10">
+      <c r="B22" s="11">
         <v>19</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" ht="13.5" spans="2:3">
-      <c r="B23" s="10">
+      <c r="B23" s="11">
         <v>20</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="24" ht="13.5" spans="2:3">
-      <c r="B24" s="10">
+      <c r="B24" s="11">
         <v>21</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="25" ht="13.5" spans="2:3">
-      <c r="B25" s="10">
+      <c r="B25" s="11">
         <v>22</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="26" ht="13.5" spans="2:3">
-      <c r="B26" s="10">
+      <c r="B26" s="11">
         <v>23</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" ht="13.5" spans="2:3">
-      <c r="B27" s="10">
+      <c r="B27" s="11">
         <v>24</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" ht="13.5" spans="2:3">
-      <c r="B28" s="10">
+      <c r="B28" s="11">
         <v>25</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="29" ht="13.5" spans="2:3">
-      <c r="B29" s="10">
+      <c r="B29" s="11">
         <v>26</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="30" ht="13.5" spans="2:3">
-      <c r="B30" s="10">
+      <c r="B30" s="11">
         <v>27</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="31" ht="13.5" spans="2:3">
-      <c r="B31" s="10">
+      <c r="B31" s="11">
         <v>28</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="32" ht="13.5" spans="2:3">
-      <c r="B32" s="10">
+      <c r="B32" s="11">
         <v>29</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" ht="13.5" spans="2:3">
-      <c r="B33" s="10">
+      <c r="B33" s="11">
         <v>30</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="34" ht="13.5" spans="2:3">
-      <c r="B34" s="10">
+      <c r="B34" s="11">
         <v>31</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="35" ht="13.5" spans="2:3">
-      <c r="B35" s="10">
+      <c r="B35" s="11">
         <v>32</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="36" ht="13.5" spans="2:3">
-      <c r="B36" s="10">
+      <c r="B36" s="11">
         <v>33</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="37" ht="13.5" spans="2:3">
-      <c r="B37" s="10">
+      <c r="B37" s="11">
         <v>34</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="38" ht="13.5" spans="2:3">
-      <c r="B38" s="10">
+      <c r="B38" s="11">
         <v>35</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="39" ht="13.5" spans="2:3">
-      <c r="B39" s="10">
+      <c r="B39" s="11">
         <v>36</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" ht="13.5" spans="2:3">
-      <c r="B40" s="10">
+      <c r="B40" s="11">
         <v>37</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="41" ht="13.5" spans="2:3">
-      <c r="B41" s="10">
+      <c r="B41" s="11">
         <v>38</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="42" ht="13.5" spans="2:3">
-      <c r="B42" s="10">
+      <c r="B42" s="11">
         <v>39</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="43" ht="13.5" spans="2:3">
-      <c r="B43" s="10">
+      <c r="B43" s="11">
         <v>40</v>
       </c>
-      <c r="C43" s="13"/>
+      <c r="C43" s="14"/>
     </row>
     <row r="44" ht="13.5" spans="2:3">
-      <c r="B44" s="10">
+      <c r="B44" s="11">
         <v>41</v>
       </c>
-      <c r="C44" s="13"/>
+      <c r="C44" s="14"/>
     </row>
     <row r="45" ht="13.5" spans="2:3">
-      <c r="B45" s="10">
+      <c r="B45" s="11">
         <v>42</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="15" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="46" ht="13.5" spans="2:3">
-      <c r="B46" s="10">
+      <c r="B46" s="11">
         <v>43</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="47" ht="13.5" spans="2:3">
-      <c r="B47" s="10">
+      <c r="B47" s="11">
         <v>44</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="48" ht="13.5" spans="2:3">
-      <c r="B48" s="10">
+      <c r="B48" s="11">
         <v>45</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="49" ht="13.5" spans="2:3">
-      <c r="B49" s="10">
+      <c r="B49" s="11">
         <v>46</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="50" ht="13.5" spans="2:3">
-      <c r="B50" s="10">
+      <c r="B50" s="11">
         <v>47</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="12" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51" ht="13.5" spans="2:3">
-      <c r="B51" s="10">
+      <c r="B51" s="11">
         <v>48</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="52" ht="13.5" spans="2:3">
-      <c r="B52" s="10">
+      <c r="B52" s="11">
         <v>49</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="53" ht="13.5" spans="2:3">
-      <c r="B53" s="10">
+      <c r="B53" s="11">
         <v>50</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="12" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="54" ht="13.5" spans="2:3">
-      <c r="B54" s="10">
+      <c r="B54" s="11">
         <v>51</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="55" ht="13.5" spans="2:3">
-      <c r="B55" s="10">
+      <c r="B55" s="11">
         <v>52</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="16" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="56" ht="13.5" spans="2:3">
-      <c r="B56" s="10">
+      <c r="B56" s="11">
         <v>53</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="16" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="57" ht="13.5" spans="2:3">
-      <c r="B57" s="10">
+      <c r="B57" s="11">
         <v>54</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="16" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="58" ht="13.5" spans="2:3">
-      <c r="B58" s="10">
+      <c r="B58" s="11">
         <v>55</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="16" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="59" ht="13.5" spans="2:3">
-      <c r="B59" s="10">
+      <c r="B59" s="11">
         <v>56</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="16" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="60" ht="13.5" spans="2:3">
-      <c r="B60" s="10">
+      <c r="B60" s="11">
         <v>57</v>
       </c>
-      <c r="C60" s="16"/>
+      <c r="C60" s="17"/>
     </row>
     <row r="61" ht="13.5" spans="2:3">
-      <c r="B61" s="10">
+      <c r="B61" s="11">
         <v>58</v>
       </c>
-      <c r="C61" s="17"/>
+      <c r="C61" s="18"/>
     </row>
     <row r="62" ht="13.5" spans="2:3">
-      <c r="B62" s="10">
+      <c r="B62" s="11">
         <v>59</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="19" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="63" ht="13.5" spans="2:3">
-      <c r="B63" s="10">
+      <c r="B63" s="11">
         <v>60</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="20" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="64" ht="13.5" spans="2:3">
-      <c r="B64" s="10">
+      <c r="B64" s="11">
         <v>61</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="20" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="65" ht="13.5" spans="2:3">
-      <c r="B65" s="10">
+      <c r="B65" s="11">
         <v>62</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="20" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="66" ht="13.5" spans="2:3">
-      <c r="B66" s="10">
+      <c r="B66" s="11">
         <v>63</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="20" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="67" ht="13.5" spans="2:3">
-      <c r="B67" s="10">
+      <c r="B67" s="11">
         <v>64</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="20" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="68" ht="13.5" spans="2:3">
-      <c r="B68" s="10">
+      <c r="B68" s="11">
         <v>65</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="20" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="69" ht="13.5" spans="2:3">
-      <c r="B69" s="10">
+      <c r="B69" s="11">
         <v>66</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="20" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="2:3">
-      <c r="B70" s="10">
+      <c r="B70" s="11">
         <v>67</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="2:3">
-      <c r="B71" s="10">
+      <c r="B71" s="11">
         <v>68</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="20" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="2:3">
-      <c r="B72" s="10">
+      <c r="B72" s="11">
         <v>69</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="2:3">
-      <c r="B73" s="10">
+      <c r="B73" s="11">
         <v>70</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="20" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="74" ht="13.5" spans="2:3">
-      <c r="B74" s="10">
+      <c r="B74" s="11">
         <v>71</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="20" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="75" ht="13.5" spans="2:3">
-      <c r="B75" s="10">
+      <c r="B75" s="11">
         <v>72</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="20" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="76" ht="13.5" spans="2:3">
-      <c r="B76" s="10">
+      <c r="B76" s="11">
         <v>73</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="20" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="77" ht="13.5" spans="2:3">
-      <c r="B77" s="10">
+      <c r="B77" s="11">
         <v>74</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="20" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="78" ht="13.5" spans="2:3">
-      <c r="B78" s="10">
+      <c r="B78" s="11">
         <v>75</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="20" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="79" ht="13.5" spans="2:3">
-      <c r="B79" s="10">
+      <c r="B79" s="11">
         <v>76</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="20" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="80" ht="13.5" spans="2:3">
-      <c r="B80" s="10">
+      <c r="B80" s="11">
         <v>77</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="20" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="81" ht="13.5" spans="2:3">
-      <c r="B81" s="10">
+      <c r="B81" s="11">
         <v>78</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="20" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="82" ht="13.5" spans="2:3">
-      <c r="B82" s="10">
+      <c r="B82" s="11">
         <v>79</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="20" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="83" ht="13.5" spans="2:3">
-      <c r="B83" s="10">
+      <c r="B83" s="11">
         <v>80</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="20" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="84" ht="13.5" spans="2:3">
-      <c r="B84" s="10">
+      <c r="B84" s="11">
         <v>81</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="20" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="85" ht="13.5" spans="2:3">
-      <c r="B85" s="10">
+      <c r="B85" s="11">
         <v>82</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="20" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="86" ht="13.5" spans="2:3">
-      <c r="B86" s="10">
+      <c r="B86" s="11">
         <v>83</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="20" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="87" ht="13.5" spans="2:3">
-      <c r="B87" s="10">
+      <c r="B87" s="11">
         <v>84</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="20" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="88" ht="13.5" spans="2:3">
-      <c r="B88" s="10">
+      <c r="B88" s="11">
         <v>85</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="20" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="89" ht="13.5" spans="2:3">
-      <c r="B89" s="10">
+      <c r="B89" s="11">
         <v>86</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="20" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="90" ht="13.5" spans="2:3">
-      <c r="B90" s="10">
+      <c r="B90" s="11">
         <v>87</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="20" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="2:3">
-      <c r="B91" s="10">
+      <c r="B91" s="11">
         <v>88</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="2:3">
-      <c r="B92" s="10">
+      <c r="B92" s="11">
         <v>89</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="C92" s="20" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="2:3">
-      <c r="B93" s="10">
+      <c r="B93" s="11">
         <v>90</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="20" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="2:3">
-      <c r="B94" s="10">
+      <c r="B94" s="11">
         <v>91</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="C94" s="20" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="95" ht="13.5" spans="2:3">
-      <c r="B95" s="10">
+      <c r="B95" s="11">
         <v>92</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="20" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="96" ht="13.5" spans="2:3">
-      <c r="B96" s="10">
+      <c r="B96" s="11">
         <v>93</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="20" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="97" ht="13.5" spans="2:3">
-      <c r="B97" s="10">
+      <c r="B97" s="11">
         <v>94</v>
       </c>
-      <c r="C97" s="19" t="s">
+      <c r="C97" s="20" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="98" ht="13.5" spans="2:3">
-      <c r="B98" s="10">
+      <c r="B98" s="11">
         <v>95</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="20" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="99" ht="13.5" spans="2:3">
-      <c r="B99" s="10">
+      <c r="B99" s="11">
         <v>96</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="20" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="100" ht="13.5" spans="2:3">
-      <c r="B100" s="10">
+      <c r="B100" s="11">
         <v>97</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="C100" s="20" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="101" ht="13.5" spans="2:3">
-      <c r="B101" s="10">
+      <c r="B101" s="11">
         <v>98</v>
       </c>
-      <c r="C101" s="13"/>
+      <c r="C101" s="14"/>
     </row>
     <row r="102" ht="13.5" spans="2:3">
-      <c r="B102" s="10">
+      <c r="B102" s="11">
         <v>99</v>
       </c>
-      <c r="C102" s="13"/>
+      <c r="C102" s="14"/>
     </row>
     <row r="103" ht="13.5" spans="2:3">
-      <c r="B103" s="10">
+      <c r="B103" s="11">
         <v>100</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" s="15" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="104" ht="13.5" spans="2:3">
-      <c r="B104" s="10">
+      <c r="B104" s="11">
         <v>101</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="12" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="105" ht="13.5" spans="2:3">
-      <c r="B105" s="10">
+      <c r="B105" s="11">
         <v>102</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="C105" s="13" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="106" ht="13.5" spans="2:3">
-      <c r="B106" s="10">
+      <c r="B106" s="11">
         <v>103</v>
       </c>
-      <c r="C106" s="12" t="s">
+      <c r="C106" s="13" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="107" ht="13.5" spans="2:3">
-      <c r="B107" s="10">
+      <c r="B107" s="11">
         <v>104</v>
       </c>
-      <c r="C107" s="12" t="s">
+      <c r="C107" s="13" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="108" ht="13.5" spans="2:3">
-      <c r="B108" s="10">
+      <c r="B108" s="11">
         <v>105</v>
       </c>
-      <c r="C108" s="12" t="s">
+      <c r="C108" s="13" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="109" ht="13.5" spans="2:3">
-      <c r="B109" s="10">
+      <c r="B109" s="11">
         <v>106</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="C109" s="13" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="110" ht="13.5" spans="2:3">
-      <c r="B110" s="10">
+      <c r="B110" s="11">
         <v>107</v>
       </c>
-      <c r="C110" s="12" t="s">
+      <c r="C110" s="13" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="111" ht="13.5" spans="2:3">
-      <c r="B111" s="10">
+      <c r="B111" s="11">
         <v>108</v>
       </c>
-      <c r="C111" s="12" t="s">
+      <c r="C111" s="13" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="112" ht="13.5" spans="2:3">
-      <c r="B112" s="10">
+      <c r="B112" s="11">
         <v>109</v>
       </c>
-      <c r="C112" s="12" t="s">
+      <c r="C112" s="13" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="113" ht="13.5" spans="2:3">
-      <c r="B113" s="10">
+      <c r="B113" s="11">
         <v>110</v>
       </c>
-      <c r="C113" s="12" t="s">
+      <c r="C113" s="13" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="114" ht="13.5" spans="2:3">
-      <c r="B114" s="10">
+      <c r="B114" s="11">
         <v>111</v>
       </c>
-      <c r="C114" s="12" t="s">
+      <c r="C114" s="13" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="115" ht="13.5" spans="2:3">
-      <c r="B115" s="10">
+      <c r="B115" s="11">
         <v>112</v>
       </c>
-      <c r="C115" s="12" t="s">
+      <c r="C115" s="13" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="116" ht="13.5" spans="2:3">
-      <c r="B116" s="10">
+      <c r="B116" s="11">
         <v>113</v>
       </c>
-      <c r="C116" s="12" t="s">
+      <c r="C116" s="13" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="117" ht="13.5" spans="2:3">
-      <c r="B117" s="10">
+      <c r="B117" s="11">
         <v>114</v>
       </c>
-      <c r="C117" s="12" t="s">
+      <c r="C117" s="13" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="118" ht="13.5" spans="2:3">
-      <c r="B118" s="10">
+      <c r="B118" s="11">
         <v>115</v>
       </c>
-      <c r="C118" s="20" t="s">
+      <c r="C118" s="21" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="119" ht="13.5" spans="2:3">
-      <c r="B119" s="10">
+      <c r="B119" s="11">
         <v>116</v>
       </c>
-      <c r="C119" s="20" t="s">
+      <c r="C119" s="21" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="120" ht="13.5" spans="2:3">
-      <c r="B120" s="10">
+      <c r="B120" s="11">
         <v>117</v>
       </c>
-      <c r="C120" s="20" t="s">
+      <c r="C120" s="21" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="121" ht="13.5" spans="2:3">
-      <c r="B121" s="10">
+      <c r="B121" s="11">
         <v>118</v>
       </c>
-      <c r="C121" s="20" t="s">
+      <c r="C121" s="21" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="122" ht="13.5" spans="2:3">
-      <c r="B122" s="10">
+      <c r="B122" s="11">
         <v>119</v>
       </c>
-      <c r="C122" s="20" t="s">
+      <c r="C122" s="21" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="123" ht="13.5" spans="2:3">
-      <c r="B123" s="10">
+      <c r="B123" s="11">
         <v>120</v>
       </c>
-      <c r="C123" s="20" t="s">
+      <c r="C123" s="21" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="124" ht="13.5" spans="2:3">
-      <c r="B124" s="10">
+      <c r="B124" s="11">
         <v>121</v>
       </c>
-      <c r="C124" s="20" t="s">
+      <c r="C124" s="21" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="125" ht="13.5" spans="2:3">
-      <c r="B125" s="10">
+      <c r="B125" s="11">
         <v>122</v>
       </c>
-      <c r="C125" s="20" t="s">
+      <c r="C125" s="21" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="126" ht="13.5" spans="2:3">
-      <c r="B126" s="10">
+      <c r="B126" s="11">
         <v>123</v>
       </c>
-      <c r="C126" s="20" t="s">
+      <c r="C126" s="21" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="127" ht="13.5" spans="2:3">
-      <c r="B127" s="10">
+      <c r="B127" s="11">
         <v>124</v>
       </c>
-      <c r="C127" s="20" t="s">
+      <c r="C127" s="21" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="128" ht="13.5" spans="2:3">
-      <c r="B128" s="10">
+      <c r="B128" s="11">
         <v>125</v>
       </c>
-      <c r="C128" s="20" t="s">
+      <c r="C128" s="21" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="129" ht="13.5" spans="2:3">
-      <c r="B129" s="10">
+      <c r="B129" s="11">
         <v>126</v>
       </c>
-      <c r="C129" s="20" t="s">
+      <c r="C129" s="21" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="130" ht="13.5" spans="2:3">
-      <c r="B130" s="10">
+      <c r="B130" s="11">
         <v>127</v>
       </c>
-      <c r="C130" s="20" t="s">
+      <c r="C130" s="21" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="131" ht="13.5" spans="2:3">
-      <c r="B131" s="10">
+      <c r="B131" s="11">
         <v>128</v>
       </c>
-      <c r="C131" s="20" t="s">
+      <c r="C131" s="21" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="132" ht="13.5" spans="2:3">
-      <c r="B132" s="10">
+      <c r="B132" s="11">
         <v>129</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C132" s="12" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="133" ht="13.5" spans="2:3">
-      <c r="B133" s="10">
+      <c r="B133" s="11">
         <v>130</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="12" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="134" ht="13.5" spans="2:3">
-      <c r="B134" s="10">
+      <c r="B134" s="11">
         <v>131</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C134" s="12" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="135" ht="13.5" spans="2:3">
-      <c r="B135" s="10">
+      <c r="B135" s="11">
         <v>132</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="12" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="136" ht="13.5" spans="2:3">
-      <c r="B136" s="10">
+      <c r="B136" s="11">
         <v>133</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="12" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="137" ht="13.5" spans="2:3">
-      <c r="B137" s="10">
+      <c r="B137" s="11">
         <v>134</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C137" s="16" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="138" ht="13.5" spans="2:3">
-      <c r="B138" s="10">
+      <c r="B138" s="11">
         <v>135</v>
       </c>
-      <c r="C138" s="15" t="s">
+      <c r="C138" s="16" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="139" ht="13.5" spans="2:3">
-      <c r="B139" s="10">
+      <c r="B139" s="11">
         <v>136</v>
       </c>
-      <c r="C139" s="15" t="s">
+      <c r="C139" s="16" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="140" ht="13.5" spans="2:3">
-      <c r="B140" s="10">
+      <c r="B140" s="11">
         <v>137</v>
       </c>
-      <c r="C140" s="21" t="s">
+      <c r="C140" s="22" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="141" ht="13.5" spans="2:3">
-      <c r="B141" s="10">
+      <c r="B141" s="11">
         <v>138</v>
       </c>
-      <c r="C141" s="21" t="s">
+      <c r="C141" s="22" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="142" ht="13.5" spans="2:3">
-      <c r="B142" s="10">
+      <c r="B142" s="11">
         <v>139</v>
       </c>
-      <c r="C142" s="21" t="s">
+      <c r="C142" s="22" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="143" ht="13.5" spans="2:3">
-      <c r="B143" s="10">
+      <c r="B143" s="11">
         <v>140</v>
       </c>
-      <c r="C143" s="21" t="s">
+      <c r="C143" s="22" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="144" ht="13.5" spans="2:3">
-      <c r="B144" s="10">
+      <c r="B144" s="11">
         <v>141</v>
       </c>
-      <c r="C144" s="21" t="s">
+      <c r="C144" s="22" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="145" ht="13.5" spans="2:3">
-      <c r="B145" s="10">
+      <c r="B145" s="11">
         <v>142</v>
       </c>
-      <c r="C145" s="21" t="s">
+      <c r="C145" s="22" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="146" ht="13.5" spans="2:3">
-      <c r="B146" s="10">
+      <c r="B146" s="11">
         <v>143</v>
       </c>
-      <c r="C146" s="21" t="s">
+      <c r="C146" s="22" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="147" ht="13.5" spans="2:3">
-      <c r="B147" s="10">
+      <c r="B147" s="11">
         <v>144</v>
       </c>
-      <c r="C147" s="21" t="s">
+      <c r="C147" s="22" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="148" ht="13.5" spans="2:3">
-      <c r="B148" s="10">
+      <c r="B148" s="11">
         <v>145</v>
       </c>
-      <c r="C148" s="21" t="s">
+      <c r="C148" s="22" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="149" ht="13.5" spans="2:3">
-      <c r="B149" s="10">
+      <c r="B149" s="11">
         <v>146</v>
       </c>
-      <c r="C149" s="22" t="s">
+      <c r="C149" s="23" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="150" ht="13.5" spans="2:3">
-      <c r="B150" s="10">
+      <c r="B150" s="11">
         <v>147</v>
       </c>
-      <c r="C150" s="12" t="s">
+      <c r="C150" s="13" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="151" ht="13.5" spans="2:3">
-      <c r="B151" s="10">
+      <c r="B151" s="11">
         <v>148</v>
       </c>
-      <c r="C151" s="12" t="s">
+      <c r="C151" s="13" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="152" ht="13.5" spans="2:3">
-      <c r="B152" s="10">
+      <c r="B152" s="11">
         <v>149</v>
       </c>
-      <c r="C152" s="12" t="s">
+      <c r="C152" s="13" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="153" ht="13.5" spans="2:3">
-      <c r="B153" s="10">
+      <c r="B153" s="11">
         <v>150</v>
       </c>
-      <c r="C153" s="13"/>
+      <c r="C153" s="14"/>
     </row>
     <row r="154" ht="13.5" spans="2:3">
-      <c r="B154" s="10">
+      <c r="B154" s="11">
         <v>151</v>
       </c>
-      <c r="C154" s="13"/>
+      <c r="C154" s="14"/>
     </row>
     <row r="155" ht="13.5" spans="2:3">
-      <c r="B155" s="10">
+      <c r="B155" s="11">
         <v>152</v>
       </c>
-      <c r="C155" s="23" t="s">
+      <c r="C155" s="24" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="156" ht="13.5" spans="2:3">
-      <c r="B156" s="10">
+      <c r="B156" s="11">
         <v>153</v>
       </c>
-      <c r="C156" s="22" t="s">
+      <c r="C156" s="23" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="157" ht="13.5" spans="2:3">
-      <c r="B157" s="10">
+      <c r="B157" s="11">
         <v>154</v>
       </c>
-      <c r="C157" s="22" t="s">
+      <c r="C157" s="23" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="158" ht="13.5" spans="2:3">
-      <c r="B158" s="10">
+      <c r="B158" s="11">
         <v>155</v>
       </c>
-      <c r="C158" s="22" t="s">
+      <c r="C158" s="23" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="159" ht="13.5" spans="2:3">
-      <c r="B159" s="10">
+      <c r="B159" s="11">
         <v>156</v>
       </c>
-      <c r="C159" s="22" t="s">
+      <c r="C159" s="23" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="160" ht="13.5" spans="2:3">
-      <c r="B160" s="10">
+      <c r="B160" s="11">
         <v>157</v>
       </c>
-      <c r="C160" s="22" t="s">
+      <c r="C160" s="23" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="161" ht="13.5" spans="2:3">
-      <c r="B161" s="10">
+      <c r="B161" s="11">
         <v>158</v>
       </c>
-      <c r="C161" s="22" t="s">
+      <c r="C161" s="23" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="162" ht="13.5" spans="2:3">
-      <c r="B162" s="10">
+      <c r="B162" s="11">
         <v>159</v>
       </c>
-      <c r="C162" s="22" t="s">
+      <c r="C162" s="23" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="163" ht="13.5" spans="2:3">
-      <c r="B163" s="10">
+      <c r="B163" s="11">
         <v>160</v>
       </c>
-      <c r="C163" s="22" t="s">
+      <c r="C163" s="23" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="164" ht="13.5" spans="2:3">
-      <c r="B164" s="10">
+      <c r="B164" s="11">
         <v>161</v>
       </c>
-      <c r="C164" s="22" t="s">
+      <c r="C164" s="23" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="165" ht="13.5" spans="2:3">
-      <c r="B165" s="10">
+      <c r="B165" s="11">
         <v>162</v>
       </c>
-      <c r="C165" s="22" t="s">
+      <c r="C165" s="23" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="166" ht="13.5" spans="2:3">
-      <c r="B166" s="10">
+      <c r="B166" s="11">
         <v>163</v>
       </c>
-      <c r="C166" s="22" t="s">
+      <c r="C166" s="23" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="167" ht="13.5" spans="2:3">
-      <c r="B167" s="10">
+      <c r="B167" s="11">
         <v>164</v>
       </c>
-      <c r="C167" s="22" t="s">
+      <c r="C167" s="23" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="168" ht="13.5" spans="2:3">
-      <c r="B168" s="10">
+      <c r="B168" s="11">
         <v>165</v>
       </c>
-      <c r="C168" s="22" t="s">
+      <c r="C168" s="23" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="169" ht="13.5" spans="2:3">
-      <c r="B169" s="10">
+      <c r="B169" s="11">
         <v>166</v>
       </c>
-      <c r="C169" s="13"/>
+      <c r="C169" s="14"/>
     </row>
     <row r="170" ht="13.5" spans="2:3">
-      <c r="B170" s="10">
+      <c r="B170" s="11">
         <v>167</v>
       </c>
-      <c r="C170" s="17"/>
+      <c r="C170" s="18"/>
     </row>
     <row r="171" ht="13.5" spans="2:3">
-      <c r="B171" s="10">
+      <c r="B171" s="11">
         <v>168</v>
       </c>
-      <c r="C171" s="18" t="s">
+      <c r="C171" s="19" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="172" ht="13.5" spans="2:3">
-      <c r="B172" s="10">
+      <c r="B172" s="11">
         <v>169</v>
       </c>
-      <c r="C172" s="11" t="s">
+      <c r="C172" s="12" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="173" ht="13.5" spans="2:3">
-      <c r="B173" s="10">
+      <c r="B173" s="11">
         <v>170</v>
       </c>
-      <c r="C173" s="11" t="s">
+      <c r="C173" s="12" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="174" ht="13.5" spans="2:3">
-      <c r="B174" s="10">
+      <c r="B174" s="11">
         <v>171</v>
       </c>
-      <c r="C174" s="11" t="s">
+      <c r="C174" s="12" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="175" ht="13.5" spans="2:3">
-      <c r="B175" s="10">
+      <c r="B175" s="11">
         <v>172</v>
       </c>
-      <c r="C175" s="11" t="s">
+      <c r="C175" s="12" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="176" ht="13.5" spans="2:3">
-      <c r="B176" s="10">
+      <c r="B176" s="11">
         <v>173</v>
       </c>
-      <c r="C176" s="11" t="s">
+      <c r="C176" s="12" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="177" ht="13.5" spans="2:3">
-      <c r="B177" s="10">
+      <c r="B177" s="11">
         <v>174</v>
       </c>
-      <c r="C177" s="11" t="s">
+      <c r="C177" s="12" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="178" ht="13.5" spans="2:3">
-      <c r="B178" s="10">
+      <c r="B178" s="11">
         <v>175</v>
       </c>
-      <c r="C178" s="11" t="s">
+      <c r="C178" s="12" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="179" ht="13.5" spans="2:3">
-      <c r="B179" s="10">
+      <c r="B179" s="11">
         <v>176</v>
       </c>
-      <c r="C179" s="11" t="s">
+      <c r="C179" s="12" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="180" ht="13.5" spans="2:3">
-      <c r="B180" s="10">
+      <c r="B180" s="11">
         <v>177</v>
       </c>
-      <c r="C180" s="11" t="s">
+      <c r="C180" s="12" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="181" ht="13.5" spans="2:3">
-      <c r="B181" s="10">
+      <c r="B181" s="11">
         <v>178</v>
       </c>
-      <c r="C181" s="11" t="s">
+      <c r="C181" s="12" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="182" ht="13.5" spans="2:3">
-      <c r="B182" s="10">
+      <c r="B182" s="11">
         <v>179</v>
       </c>
-      <c r="C182" s="11" t="s">
+      <c r="C182" s="12" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="183" ht="13.5" spans="2:3">
-      <c r="B183" s="10">
+      <c r="B183" s="11">
         <v>180</v>
       </c>
-      <c r="C183" s="11" t="s">
+      <c r="C183" s="12" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="184" ht="13.5" spans="2:3">
-      <c r="B184" s="10">
+      <c r="B184" s="11">
         <v>181</v>
       </c>
-      <c r="C184" s="11" t="s">
+      <c r="C184" s="12" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="185" ht="13.5" spans="2:3">
-      <c r="B185" s="10">
+      <c r="B185" s="11">
         <v>182</v>
       </c>
-      <c r="C185" s="11" t="s">
+      <c r="C185" s="12" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="186" ht="13.5" spans="2:3">
-      <c r="B186" s="10">
+      <c r="B186" s="11">
         <v>183</v>
       </c>
-      <c r="C186" s="11" t="s">
+      <c r="C186" s="12" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="187" ht="13.5" spans="2:3">
-      <c r="B187" s="10">
+      <c r="B187" s="11">
         <v>184</v>
       </c>
-      <c r="C187" s="11" t="s">
+      <c r="C187" s="12" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="188" ht="13.5" spans="2:3">
-      <c r="B188" s="10">
+      <c r="B188" s="11">
         <v>185</v>
       </c>
-      <c r="C188" s="13"/>
+      <c r="C188" s="14"/>
     </row>
     <row r="189" ht="13.5" spans="2:3">
-      <c r="B189" s="10">
+      <c r="B189" s="11">
         <v>186</v>
       </c>
-      <c r="C189" s="13"/>
+      <c r="C189" s="14"/>
     </row>
     <row r="190" ht="13.5" spans="2:3">
-      <c r="B190" s="10">
+      <c r="B190" s="11">
         <v>187</v>
       </c>
-      <c r="C190" s="18" t="s">
+      <c r="C190" s="19" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="191" ht="13.5" spans="2:3">
-      <c r="B191" s="10">
+      <c r="B191" s="11">
         <v>188</v>
       </c>
-      <c r="C191" s="11" t="s">
+      <c r="C191" s="12" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="192" ht="13.5" spans="2:3">
-      <c r="B192" s="10">
+      <c r="B192" s="11">
         <v>189</v>
       </c>
-      <c r="C192" s="11" t="s">
+      <c r="C192" s="12" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="193" ht="13.5" spans="2:3">
-      <c r="B193" s="10">
+      <c r="B193" s="11">
         <v>190</v>
       </c>
-      <c r="C193" s="11" t="s">
+      <c r="C193" s="12" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="194" ht="13.5" spans="2:3">
-      <c r="B194" s="10">
+      <c r="B194" s="11">
         <v>191</v>
       </c>
-      <c r="C194" s="11" t="s">
+      <c r="C194" s="12" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="195" ht="13.5" spans="2:3">
-      <c r="B195" s="10">
+      <c r="B195" s="11">
         <v>192</v>
       </c>
-      <c r="C195" s="11" t="s">
+      <c r="C195" s="12" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="196" ht="13.5" spans="2:3">
-      <c r="B196" s="10">
+      <c r="B196" s="11">
         <v>193</v>
       </c>
-      <c r="C196" s="11" t="s">
+      <c r="C196" s="12" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="197" ht="13.5" spans="2:3">
-      <c r="B197" s="10">
+      <c r="B197" s="11">
         <v>194</v>
       </c>
-      <c r="C197" s="11" t="s">
+      <c r="C197" s="12" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="198" ht="13.5" spans="2:3">
-      <c r="B198" s="10">
+      <c r="B198" s="11">
         <v>195</v>
       </c>
-      <c r="C198" s="11" t="s">
+      <c r="C198" s="12" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="199" ht="13.5" spans="2:3">
-      <c r="B199" s="10">
+      <c r="B199" s="11">
         <v>196</v>
       </c>
-      <c r="C199" s="17"/>
+      <c r="C199" s="18"/>
     </row>
     <row r="200" ht="13.5" spans="2:3">
-      <c r="B200" s="10">
+      <c r="B200" s="11">
         <v>197</v>
       </c>
-      <c r="C200" s="17"/>
+      <c r="C200" s="18"/>
     </row>
     <row r="201" ht="13.5" spans="2:3">
-      <c r="B201" s="10">
+      <c r="B201" s="11">
         <v>198</v>
       </c>
-      <c r="C201" s="18" t="s">
+      <c r="C201" s="19" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="202" ht="13.5" spans="2:3">
-      <c r="B202" s="10">
+      <c r="B202" s="11">
         <v>199</v>
       </c>
-      <c r="C202" s="11" t="s">
+      <c r="C202" s="12" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="203" ht="13.5" spans="2:3">
-      <c r="B203" s="10">
+      <c r="B203" s="11">
         <v>200</v>
       </c>
-      <c r="C203" s="11" t="s">
+      <c r="C203" s="12" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="204" ht="13.5" spans="2:3">
-      <c r="B204" s="10">
+      <c r="B204" s="11">
         <v>201</v>
       </c>
-      <c r="C204" s="11" t="s">
+      <c r="C204" s="12" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="205" ht="13.5" spans="2:3">
-      <c r="B205" s="10">
+      <c r="B205" s="11">
         <v>202</v>
       </c>
-      <c r="C205" s="11" t="s">
+      <c r="C205" s="12" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="206" ht="13.5" spans="2:3">
-      <c r="B206" s="10">
+      <c r="B206" s="11">
         <v>203</v>
       </c>
-      <c r="C206" s="11" t="s">
+      <c r="C206" s="12" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="207" ht="13.5" spans="2:3">
-      <c r="B207" s="10">
+      <c r="B207" s="11">
         <v>204</v>
       </c>
-      <c r="C207" s="11" t="s">
+      <c r="C207" s="12" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="208" ht="13.5" spans="2:3">
-      <c r="B208" s="10">
+      <c r="B208" s="11">
         <v>205</v>
       </c>
-      <c r="C208" s="11" t="s">
+      <c r="C208" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="209" ht="13.5" spans="2:3">
-      <c r="B209" s="10">
+      <c r="B209" s="11">
         <v>206</v>
       </c>
-      <c r="C209" s="17"/>
+      <c r="C209" s="18"/>
     </row>
     <row r="210" ht="13.5" spans="2:3">
-      <c r="B210" s="10">
+      <c r="B210" s="11">
         <v>207</v>
       </c>
-      <c r="C210" s="17"/>
+      <c r="C210" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4368,21 +4442,21 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" ht="27" customHeight="1" spans="1:13">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="1" t="s">
@@ -4391,52 +4465,52 @@
       <c r="F3" t="s">
         <v>245</v>
       </c>
-      <c r="O3" s="8"/>
+      <c r="O3" s="9"/>
       <c r="Q3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="4" spans="15:15">
-      <c r="O4" s="8"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="3:15">
       <c r="C5" t="s">
         <v>247</v>
       </c>
-      <c r="O5" s="8"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="15:15">
-      <c r="O6" s="8"/>
+      <c r="O6" s="9"/>
     </row>
     <row r="7" spans="5:15">
       <c r="E7" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="O7" s="8"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="6:15">
       <c r="F8" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="O8" s="8"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" spans="6:15">
       <c r="F9" t="s">
         <v>250</v>
       </c>
-      <c r="O9" s="8"/>
+      <c r="O9" s="9"/>
     </row>
     <row r="10" spans="6:15">
       <c r="F10" t="s">
         <v>251</v>
       </c>
-      <c r="O10" s="8"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="15:15">
-      <c r="O11" s="8"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="15:15">
-      <c r="O12" s="8"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
@@ -4489,10 +4563,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:L54"/>
+  <dimension ref="A2:L66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65:G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14.25"/>
@@ -4584,7 +4658,7 @@
       <c r="C45" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I45" s="6"/>
+      <c r="I45" s="7"/>
       <c r="K45" t="s">
         <v>276</v>
       </c>
@@ -4593,10 +4667,10 @@
       <c r="C46" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="I46" s="6"/>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" spans="9:12">
-      <c r="I47" s="6"/>
+      <c r="I47" s="7"/>
       <c r="L47" s="1" t="s">
         <v>278</v>
       </c>
@@ -4605,34 +4679,74 @@
       <c r="B48" t="s">
         <v>279</v>
       </c>
-      <c r="I48" s="6"/>
+      <c r="I48" s="7"/>
     </row>
     <row r="49" spans="3:9">
       <c r="C49" t="s">
         <v>280</v>
       </c>
-      <c r="I49" s="6"/>
-    </row>
-    <row r="50" spans="9:9">
-      <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="9:9">
-      <c r="I51" s="6"/>
-    </row>
-    <row r="52" spans="2:9">
-      <c r="B52" t="s">
+      <c r="I49" s="7"/>
+    </row>
+    <row r="52" ht="15.75" spans="3:9">
+      <c r="C52" t="s">
         <v>281</v>
       </c>
-      <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="3:9">
+      <c r="H52" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" ht="15.75" spans="3:9">
       <c r="C53" t="s">
-        <v>282</v>
-      </c>
-      <c r="I53" s="6"/>
-    </row>
-    <row r="54" spans="9:9">
-      <c r="I54" s="6"/>
+        <v>283</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" ht="15.75" spans="3:9">
+      <c r="C54" t="s">
+        <v>285</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" ht="15.75" spans="3:9">
+      <c r="C55" t="s">
+        <v>287</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" t="s">
+        <v>293</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4646,115 +4760,115 @@
   <sheetPr/>
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:C36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4762,4 +4876,76 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B2:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3">
+      <c r="C4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3">
+      <c r="C6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3">
+      <c r="C10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3">
+      <c r="C12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
+      <c r="C16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agrego algunas librerias jcalendar y jfreechart
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="9555" tabRatio="916" activeTab="4"/>
+    <workbookView windowWidth="23955" windowHeight="9735" tabRatio="916" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NECESIDADES" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="332">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -950,6 +950,24 @@
     <t>https://github.com/chenaoh/curso-java-swing-codejavu</t>
   </si>
   <si>
+    <t>JCALENDAR:</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=av8C2VmAGqo</t>
+  </si>
+  <si>
+    <t>video explicativo para instalar jcalendar en java netbeans</t>
+  </si>
+  <si>
+    <t>https://toedter.com/jcalendar/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codigo fuente del jcalendar: </t>
+  </si>
+  <si>
+    <t>https://github.com/javatlacati/jcalendar</t>
+  </si>
+  <si>
     <t>Añadorr al fichero pom.xml</t>
   </si>
   <si>
@@ -1051,10 +1069,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -1117,6 +1135,26 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1125,13 +1163,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1139,14 +1172,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1170,14 +1203,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1191,6 +1217,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1199,8 +1231,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1214,59 +1283,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1340,114 +1358,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1460,7 +1370,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1472,13 +1430,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1490,7 +1484,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1502,13 +1526,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1577,17 +1595,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1607,17 +1646,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1633,170 +1672,149 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4563,10 +4581,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:L66"/>
+  <dimension ref="A2:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:G68"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14.25"/>
@@ -4738,6 +4756,9 @@
         <v>291</v>
       </c>
     </row>
+    <row r="62" ht="12.75"/>
+    <row r="63" ht="12.75"/>
+    <row r="64" ht="12.75"/>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>292</v>
@@ -4746,6 +4767,33 @@
     <row r="66" spans="3:3">
       <c r="C66" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="67" ht="12.75"/>
+    <row r="69" spans="2:2">
+      <c r="B69" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9">
+      <c r="C70" t="s">
+        <v>295</v>
+      </c>
+      <c r="I70" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9">
+      <c r="C71" t="s">
+        <v>297</v>
+      </c>
+      <c r="I71" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -4768,107 +4816,107 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -4891,57 +4939,57 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
imprimir reporte (desde fuera del IDE)
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="9555" tabRatio="916" activeTab="1"/>
+    <workbookView windowWidth="23955" windowHeight="9735" tabRatio="916" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NECESIDADES" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="338">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -166,61 +166,64 @@
     <t>varchar</t>
   </si>
   <si>
+    <t>Venta</t>
+  </si>
+  <si>
+    <t>idventa</t>
+  </si>
+  <si>
+    <t>total pvp</t>
+  </si>
+  <si>
+    <t>total coste</t>
+  </si>
+  <si>
+    <t>total iva</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [tendero/venta]</t>
+  </si>
+  <si>
+    <t>ListaVenta</t>
+  </si>
+  <si>
     <t>IDproducto</t>
   </si>
   <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>origen</t>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>pvp unitario</t>
+  </si>
+  <si>
+    <t>coste unitario</t>
+  </si>
+  <si>
+    <t>CADENA</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>producto</t>
   </si>
   <si>
     <t>[entradas o salidas, se diferencia de valores signo (+) entrada y (-) salidas (ventas, roturas, robos, etc)</t>
   </si>
   <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>texto</t>
-  </si>
-  <si>
     <t>Positivo (+) compra</t>
   </si>
   <si>
+    <t>Idproducto</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
     <t>Negativo (-) venta, rotura, robo</t>
-  </si>
-  <si>
-    <t>VENTA</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>PVC</t>
-  </si>
-  <si>
-    <t>COSTE</t>
-  </si>
-  <si>
-    <t>FECHA</t>
-  </si>
-  <si>
-    <t>TOTAL PVC</t>
-  </si>
-  <si>
-    <t>TOTALCOSTE</t>
-  </si>
-  <si>
-    <t>TOTALBENEFICIO</t>
-  </si>
-  <si>
-    <t>TOTAL IVA</t>
-  </si>
-  <si>
-    <t>CADENA</t>
-  </si>
-  <si>
-    <t>FLOAT</t>
   </si>
   <si>
     <t>Código</t>
@@ -1084,10 +1087,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -1150,8 +1153,9 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1163,7 +1167,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1177,7 +1188,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1187,6 +1198,22 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1207,12 +1234,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1231,22 +1264,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -1255,7 +1272,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1269,27 +1286,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1297,11 +1293,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1373,7 +1376,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1397,13 +1400,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1415,73 +1424,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1499,19 +1448,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1523,7 +1514,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1535,13 +1526,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1601,8 +1604,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1611,7 +1614,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1627,6 +1630,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1660,8 +1678,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1680,160 +1698,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1907,27 +1910,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2584,10 +2591,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C2:L22"/>
+  <dimension ref="C2:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="C21:L22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -2656,7 +2663,7 @@
       <c r="H7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="40" t="s">
         <v>30</v>
       </c>
       <c r="J7"/>
@@ -2671,13 +2678,13 @@
       <c r="E8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="36" t="s">
         <v>33</v>
       </c>
       <c r="I8" s="29" t="s">
@@ -2700,7 +2707,7 @@
       <c r="H9" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2715,123 +2722,167 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="3:3">
-      <c r="C12" s="26" t="s">
+    <row r="13" spans="3:3">
+      <c r="C13" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8">
+      <c r="C14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8">
+      <c r="C15" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="C19" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9">
+      <c r="C24" s="26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="3:9">
-      <c r="C13" s="31" t="s">
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="34"/>
+      <c r="I25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9">
+      <c r="C26" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9">
-      <c r="C14" s="30" t="s">
+      <c r="D26" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" ht="21" spans="3:7">
+      <c r="C27" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="9:9">
-      <c r="I15" t="s">
+      <c r="E27" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="39"/>
+    </row>
+    <row r="28" spans="4:6">
+      <c r="D28" s="30">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12">
-      <c r="C21" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="K21" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="L21" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="J22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="K22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="37" t="s">
-        <v>56</v>
+      <c r="E28" s="30">
+        <v>150</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5">
+      <c r="D29" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2862,10 +2913,10 @@
     <row r="2" ht="13.5"/>
     <row r="3" ht="13.5" spans="2:3">
       <c r="B3" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" ht="13.5" spans="2:3">
@@ -2873,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" ht="13.5" spans="2:3">
@@ -2881,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" ht="13.5" spans="2:3">
@@ -2889,7 +2940,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" ht="13.5" spans="2:3">
@@ -2897,7 +2948,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" ht="13.5" spans="2:3">
@@ -2905,7 +2956,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" ht="13.5" spans="2:3">
@@ -2913,7 +2964,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" ht="13.5" spans="2:3">
@@ -2921,7 +2972,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" ht="13.5" spans="2:3">
@@ -2929,7 +2980,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" ht="13.5" spans="2:3">
@@ -2937,7 +2988,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" ht="13.5" spans="2:3">
@@ -2945,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" ht="13.5" spans="2:3">
@@ -2953,7 +3004,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" ht="13.5" spans="2:3">
@@ -2961,7 +3012,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" ht="13.5" spans="2:3">
@@ -2969,7 +3020,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" ht="13.5" spans="2:3">
@@ -2977,7 +3028,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" ht="13.5" spans="2:3">
@@ -2985,7 +3036,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" ht="13.5" spans="2:3">
@@ -2993,7 +3044,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" ht="13.5" spans="2:3">
@@ -3001,7 +3052,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" ht="13.5" spans="2:3">
@@ -3009,7 +3060,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" ht="13.5" spans="2:3">
@@ -3017,7 +3068,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" ht="13.5" spans="2:3">
@@ -3025,7 +3076,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" ht="13.5" spans="2:3">
@@ -3033,7 +3084,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" ht="13.5" spans="2:3">
@@ -3041,7 +3092,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" ht="13.5" spans="2:3">
@@ -3049,7 +3100,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" ht="13.5" spans="2:3">
@@ -3057,7 +3108,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" ht="13.5" spans="2:3">
@@ -3065,7 +3116,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" ht="13.5" spans="2:3">
@@ -3073,7 +3124,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" ht="13.5" spans="2:3">
@@ -3081,7 +3132,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" ht="13.5" spans="2:3">
@@ -3089,7 +3140,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" ht="13.5" spans="2:3">
@@ -3097,7 +3148,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" ht="13.5" spans="2:3">
@@ -3105,7 +3156,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" ht="13.5" spans="2:3">
@@ -3113,7 +3164,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" ht="13.5" spans="2:3">
@@ -3121,7 +3172,7 @@
         <v>32</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" ht="13.5" spans="2:3">
@@ -3129,7 +3180,7 @@
         <v>33</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" ht="13.5" spans="2:3">
@@ -3137,7 +3188,7 @@
         <v>34</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" ht="13.5" spans="2:3">
@@ -3145,7 +3196,7 @@
         <v>35</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" ht="13.5" spans="2:3">
@@ -3153,7 +3204,7 @@
         <v>36</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" ht="13.5" spans="2:3">
@@ -3161,7 +3212,7 @@
         <v>37</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" ht="13.5" spans="2:3">
@@ -3169,7 +3220,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" ht="13.5" spans="2:3">
@@ -3177,7 +3228,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" ht="13.5" spans="2:3">
@@ -3197,7 +3248,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" ht="13.5" spans="2:3">
@@ -3205,7 +3256,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" ht="13.5" spans="2:3">
@@ -3213,7 +3264,7 @@
         <v>44</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" ht="13.5" spans="2:3">
@@ -3221,7 +3272,7 @@
         <v>45</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" ht="13.5" spans="2:3">
@@ -3229,7 +3280,7 @@
         <v>46</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" ht="13.5" spans="2:3">
@@ -3237,7 +3288,7 @@
         <v>47</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" ht="13.5" spans="2:3">
@@ -3245,7 +3296,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" ht="13.5" spans="2:3">
@@ -3253,7 +3304,7 @@
         <v>49</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" ht="13.5" spans="2:3">
@@ -3261,7 +3312,7 @@
         <v>50</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" ht="13.5" spans="2:3">
@@ -3269,7 +3320,7 @@
         <v>51</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" ht="13.5" spans="2:3">
@@ -3277,7 +3328,7 @@
         <v>52</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" ht="13.5" spans="2:3">
@@ -3285,7 +3336,7 @@
         <v>53</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" ht="13.5" spans="2:3">
@@ -3293,7 +3344,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" ht="13.5" spans="2:3">
@@ -3301,7 +3352,7 @@
         <v>55</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" ht="13.5" spans="2:3">
@@ -3309,7 +3360,7 @@
         <v>56</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" ht="13.5" spans="2:3">
@@ -3329,7 +3380,7 @@
         <v>59</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" ht="13.5" spans="2:3">
@@ -3337,7 +3388,7 @@
         <v>60</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" ht="13.5" spans="2:3">
@@ -3345,7 +3396,7 @@
         <v>61</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" ht="13.5" spans="2:3">
@@ -3353,7 +3404,7 @@
         <v>62</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" ht="13.5" spans="2:3">
@@ -3361,7 +3412,7 @@
         <v>63</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" ht="13.5" spans="2:3">
@@ -3369,7 +3420,7 @@
         <v>64</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" ht="13.5" spans="2:3">
@@ -3377,7 +3428,7 @@
         <v>65</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" ht="13.5" spans="2:3">
@@ -3385,7 +3436,7 @@
         <v>66</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="2:3">
@@ -3393,7 +3444,7 @@
         <v>67</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="2:3">
@@ -3401,7 +3452,7 @@
         <v>68</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="2:3">
@@ -3409,7 +3460,7 @@
         <v>69</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="2:3">
@@ -3417,7 +3468,7 @@
         <v>70</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" ht="13.5" spans="2:3">
@@ -3425,7 +3476,7 @@
         <v>71</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" ht="13.5" spans="2:3">
@@ -3433,7 +3484,7 @@
         <v>72</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" ht="13.5" spans="2:3">
@@ -3441,7 +3492,7 @@
         <v>73</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" ht="13.5" spans="2:3">
@@ -3449,7 +3500,7 @@
         <v>74</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" ht="13.5" spans="2:3">
@@ -3457,7 +3508,7 @@
         <v>75</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" ht="13.5" spans="2:3">
@@ -3465,7 +3516,7 @@
         <v>76</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" ht="13.5" spans="2:3">
@@ -3473,7 +3524,7 @@
         <v>77</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" ht="13.5" spans="2:3">
@@ -3481,7 +3532,7 @@
         <v>78</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" ht="13.5" spans="2:3">
@@ -3489,7 +3540,7 @@
         <v>79</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" ht="13.5" spans="2:3">
@@ -3497,7 +3548,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" ht="13.5" spans="2:3">
@@ -3505,7 +3556,7 @@
         <v>81</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" ht="13.5" spans="2:3">
@@ -3513,7 +3564,7 @@
         <v>82</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" ht="13.5" spans="2:3">
@@ -3521,7 +3572,7 @@
         <v>83</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" ht="13.5" spans="2:3">
@@ -3529,7 +3580,7 @@
         <v>84</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" ht="13.5" spans="2:3">
@@ -3537,7 +3588,7 @@
         <v>85</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" ht="13.5" spans="2:3">
@@ -3545,7 +3596,7 @@
         <v>86</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" ht="13.5" spans="2:3">
@@ -3553,7 +3604,7 @@
         <v>87</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="2:3">
@@ -3561,7 +3612,7 @@
         <v>88</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="2:3">
@@ -3569,7 +3620,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="2:3">
@@ -3577,7 +3628,7 @@
         <v>90</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="2:3">
@@ -3585,7 +3636,7 @@
         <v>91</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" ht="13.5" spans="2:3">
@@ -3593,7 +3644,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" ht="13.5" spans="2:3">
@@ -3601,7 +3652,7 @@
         <v>93</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" ht="13.5" spans="2:3">
@@ -3609,7 +3660,7 @@
         <v>94</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" ht="13.5" spans="2:3">
@@ -3617,7 +3668,7 @@
         <v>95</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" ht="13.5" spans="2:3">
@@ -3625,7 +3676,7 @@
         <v>96</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" ht="13.5" spans="2:3">
@@ -3633,7 +3684,7 @@
         <v>97</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101" ht="13.5" spans="2:3">
@@ -3653,7 +3704,7 @@
         <v>100</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" ht="13.5" spans="2:3">
@@ -3661,7 +3712,7 @@
         <v>101</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" ht="13.5" spans="2:3">
@@ -3669,7 +3720,7 @@
         <v>102</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" ht="13.5" spans="2:3">
@@ -3677,7 +3728,7 @@
         <v>103</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="107" ht="13.5" spans="2:3">
@@ -3685,7 +3736,7 @@
         <v>104</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" ht="13.5" spans="2:3">
@@ -3693,7 +3744,7 @@
         <v>105</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="109" ht="13.5" spans="2:3">
@@ -3701,7 +3752,7 @@
         <v>106</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" ht="13.5" spans="2:3">
@@ -3709,7 +3760,7 @@
         <v>107</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111" ht="13.5" spans="2:3">
@@ -3717,7 +3768,7 @@
         <v>108</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" ht="13.5" spans="2:3">
@@ -3725,7 +3776,7 @@
         <v>109</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" ht="13.5" spans="2:3">
@@ -3733,7 +3784,7 @@
         <v>110</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" ht="13.5" spans="2:3">
@@ -3741,7 +3792,7 @@
         <v>111</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" ht="13.5" spans="2:3">
@@ -3749,7 +3800,7 @@
         <v>112</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" ht="13.5" spans="2:3">
@@ -3757,7 +3808,7 @@
         <v>113</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" ht="13.5" spans="2:3">
@@ -3765,7 +3816,7 @@
         <v>114</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118" ht="13.5" spans="2:3">
@@ -3773,7 +3824,7 @@
         <v>115</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="119" ht="13.5" spans="2:3">
@@ -3781,7 +3832,7 @@
         <v>116</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" ht="13.5" spans="2:3">
@@ -3789,7 +3840,7 @@
         <v>117</v>
       </c>
       <c r="C120" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="121" ht="13.5" spans="2:3">
@@ -3797,7 +3848,7 @@
         <v>118</v>
       </c>
       <c r="C121" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="122" ht="13.5" spans="2:3">
@@ -3805,7 +3856,7 @@
         <v>119</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="123" ht="13.5" spans="2:3">
@@ -3813,7 +3864,7 @@
         <v>120</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="124" ht="13.5" spans="2:3">
@@ -3821,7 +3872,7 @@
         <v>121</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="125" ht="13.5" spans="2:3">
@@ -3829,7 +3880,7 @@
         <v>122</v>
       </c>
       <c r="C125" s="21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126" ht="13.5" spans="2:3">
@@ -3837,7 +3888,7 @@
         <v>123</v>
       </c>
       <c r="C126" s="21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="127" ht="13.5" spans="2:3">
@@ -3845,7 +3896,7 @@
         <v>124</v>
       </c>
       <c r="C127" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="128" ht="13.5" spans="2:3">
@@ -3853,7 +3904,7 @@
         <v>125</v>
       </c>
       <c r="C128" s="21" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="129" ht="13.5" spans="2:3">
@@ -3861,7 +3912,7 @@
         <v>126</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="130" ht="13.5" spans="2:3">
@@ -3869,7 +3920,7 @@
         <v>127</v>
       </c>
       <c r="C130" s="21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" ht="13.5" spans="2:3">
@@ -3877,7 +3928,7 @@
         <v>128</v>
       </c>
       <c r="C131" s="21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" ht="13.5" spans="2:3">
@@ -3885,7 +3936,7 @@
         <v>129</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="133" ht="13.5" spans="2:3">
@@ -3893,7 +3944,7 @@
         <v>130</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="134" ht="13.5" spans="2:3">
@@ -3901,7 +3952,7 @@
         <v>131</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="135" ht="13.5" spans="2:3">
@@ -3909,7 +3960,7 @@
         <v>132</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136" ht="13.5" spans="2:3">
@@ -3917,7 +3968,7 @@
         <v>133</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="137" ht="13.5" spans="2:3">
@@ -3925,7 +3976,7 @@
         <v>134</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="138" ht="13.5" spans="2:3">
@@ -3933,7 +3984,7 @@
         <v>135</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="139" ht="13.5" spans="2:3">
@@ -3941,7 +3992,7 @@
         <v>136</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="140" ht="13.5" spans="2:3">
@@ -3949,7 +4000,7 @@
         <v>137</v>
       </c>
       <c r="C140" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="141" ht="13.5" spans="2:3">
@@ -3957,7 +4008,7 @@
         <v>138</v>
       </c>
       <c r="C141" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="142" ht="13.5" spans="2:3">
@@ -3965,7 +4016,7 @@
         <v>139</v>
       </c>
       <c r="C142" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="143" ht="13.5" spans="2:3">
@@ -3973,7 +4024,7 @@
         <v>140</v>
       </c>
       <c r="C143" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" ht="13.5" spans="2:3">
@@ -3981,7 +4032,7 @@
         <v>141</v>
       </c>
       <c r="C144" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="145" ht="13.5" spans="2:3">
@@ -3989,7 +4040,7 @@
         <v>142</v>
       </c>
       <c r="C145" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="146" ht="13.5" spans="2:3">
@@ -3997,7 +4048,7 @@
         <v>143</v>
       </c>
       <c r="C146" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="147" ht="13.5" spans="2:3">
@@ -4005,7 +4056,7 @@
         <v>144</v>
       </c>
       <c r="C147" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="148" ht="13.5" spans="2:3">
@@ -4013,7 +4064,7 @@
         <v>145</v>
       </c>
       <c r="C148" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="149" ht="13.5" spans="2:3">
@@ -4021,7 +4072,7 @@
         <v>146</v>
       </c>
       <c r="C149" s="23" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" ht="13.5" spans="2:3">
@@ -4029,7 +4080,7 @@
         <v>147</v>
       </c>
       <c r="C150" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="151" ht="13.5" spans="2:3">
@@ -4037,7 +4088,7 @@
         <v>148</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="152" ht="13.5" spans="2:3">
@@ -4045,7 +4096,7 @@
         <v>149</v>
       </c>
       <c r="C152" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="153" ht="13.5" spans="2:3">
@@ -4065,7 +4116,7 @@
         <v>152</v>
       </c>
       <c r="C155" s="24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="156" ht="13.5" spans="2:3">
@@ -4073,7 +4124,7 @@
         <v>153</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="157" ht="13.5" spans="2:3">
@@ -4081,7 +4132,7 @@
         <v>154</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="158" ht="13.5" spans="2:3">
@@ -4089,7 +4140,7 @@
         <v>155</v>
       </c>
       <c r="C158" s="23" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="159" ht="13.5" spans="2:3">
@@ -4097,7 +4148,7 @@
         <v>156</v>
       </c>
       <c r="C159" s="23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="160" ht="13.5" spans="2:3">
@@ -4105,7 +4156,7 @@
         <v>157</v>
       </c>
       <c r="C160" s="23" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="161" ht="13.5" spans="2:3">
@@ -4113,7 +4164,7 @@
         <v>158</v>
       </c>
       <c r="C161" s="23" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="162" ht="13.5" spans="2:3">
@@ -4121,7 +4172,7 @@
         <v>159</v>
       </c>
       <c r="C162" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="163" ht="13.5" spans="2:3">
@@ -4129,7 +4180,7 @@
         <v>160</v>
       </c>
       <c r="C163" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="164" ht="13.5" spans="2:3">
@@ -4137,7 +4188,7 @@
         <v>161</v>
       </c>
       <c r="C164" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="165" ht="13.5" spans="2:3">
@@ -4145,7 +4196,7 @@
         <v>162</v>
       </c>
       <c r="C165" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="166" ht="13.5" spans="2:3">
@@ -4153,7 +4204,7 @@
         <v>163</v>
       </c>
       <c r="C166" s="23" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="167" ht="13.5" spans="2:3">
@@ -4161,7 +4212,7 @@
         <v>164</v>
       </c>
       <c r="C167" s="23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="168" ht="13.5" spans="2:3">
@@ -4169,7 +4220,7 @@
         <v>165</v>
       </c>
       <c r="C168" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="169" ht="13.5" spans="2:3">
@@ -4189,7 +4240,7 @@
         <v>168</v>
       </c>
       <c r="C171" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="172" ht="13.5" spans="2:3">
@@ -4197,7 +4248,7 @@
         <v>169</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="173" ht="13.5" spans="2:3">
@@ -4205,7 +4256,7 @@
         <v>170</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="174" ht="13.5" spans="2:3">
@@ -4213,7 +4264,7 @@
         <v>171</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="175" ht="13.5" spans="2:3">
@@ -4221,7 +4272,7 @@
         <v>172</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="176" ht="13.5" spans="2:3">
@@ -4229,7 +4280,7 @@
         <v>173</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="177" ht="13.5" spans="2:3">
@@ -4237,7 +4288,7 @@
         <v>174</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="178" ht="13.5" spans="2:3">
@@ -4245,7 +4296,7 @@
         <v>175</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="179" ht="13.5" spans="2:3">
@@ -4253,7 +4304,7 @@
         <v>176</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="180" ht="13.5" spans="2:3">
@@ -4261,7 +4312,7 @@
         <v>177</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="181" ht="13.5" spans="2:3">
@@ -4269,7 +4320,7 @@
         <v>178</v>
       </c>
       <c r="C181" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="182" ht="13.5" spans="2:3">
@@ -4277,7 +4328,7 @@
         <v>179</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="183" ht="13.5" spans="2:3">
@@ -4285,7 +4336,7 @@
         <v>180</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="184" ht="13.5" spans="2:3">
@@ -4293,7 +4344,7 @@
         <v>181</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="185" ht="13.5" spans="2:3">
@@ -4301,7 +4352,7 @@
         <v>182</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="186" ht="13.5" spans="2:3">
@@ -4309,7 +4360,7 @@
         <v>183</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="187" ht="13.5" spans="2:3">
@@ -4317,7 +4368,7 @@
         <v>184</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="188" ht="13.5" spans="2:3">
@@ -4337,7 +4388,7 @@
         <v>187</v>
       </c>
       <c r="C190" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="191" ht="13.5" spans="2:3">
@@ -4345,7 +4396,7 @@
         <v>188</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="192" ht="13.5" spans="2:3">
@@ -4353,7 +4404,7 @@
         <v>189</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="193" ht="13.5" spans="2:3">
@@ -4361,7 +4412,7 @@
         <v>190</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" ht="13.5" spans="2:3">
@@ -4369,7 +4420,7 @@
         <v>191</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="195" ht="13.5" spans="2:3">
@@ -4377,7 +4428,7 @@
         <v>192</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="196" ht="13.5" spans="2:3">
@@ -4385,7 +4436,7 @@
         <v>193</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="197" ht="13.5" spans="2:3">
@@ -4393,7 +4444,7 @@
         <v>194</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="198" ht="13.5" spans="2:3">
@@ -4401,7 +4452,7 @@
         <v>195</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="199" ht="13.5" spans="2:3">
@@ -4421,7 +4472,7 @@
         <v>198</v>
       </c>
       <c r="C201" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="202" ht="13.5" spans="2:3">
@@ -4429,7 +4480,7 @@
         <v>199</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="203" ht="13.5" spans="2:3">
@@ -4437,7 +4488,7 @@
         <v>200</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="204" ht="13.5" spans="2:3">
@@ -4445,7 +4496,7 @@
         <v>201</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="205" ht="13.5" spans="2:3">
@@ -4453,7 +4504,7 @@
         <v>202</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="206" ht="13.5" spans="2:3">
@@ -4461,7 +4512,7 @@
         <v>203</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="207" ht="13.5" spans="2:3">
@@ -4469,7 +4520,7 @@
         <v>204</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="208" ht="13.5" spans="2:3">
@@ -4477,7 +4528,7 @@
         <v>205</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="209" ht="13.5" spans="2:3">
@@ -4511,7 +4562,7 @@
   <sheetData>
     <row r="1" ht="27" customHeight="1" spans="1:13">
       <c r="A1" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4528,14 +4579,14 @@
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O3" s="9"/>
       <c r="Q3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="15:15">
@@ -4543,7 +4594,7 @@
     </row>
     <row r="5" spans="3:15">
       <c r="C5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="O5" s="9"/>
     </row>
@@ -4552,25 +4603,25 @@
     </row>
     <row r="7" spans="5:15">
       <c r="E7" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="O7" s="9"/>
     </row>
     <row r="8" spans="6:15">
       <c r="F8" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="6:15">
       <c r="F9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="6:15">
       <c r="F10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="O10" s="9"/>
     </row>
@@ -4582,40 +4633,40 @@
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="16:16">
       <c r="P20" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Q21" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="4:4">
       <c r="D39" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="4:4">
       <c r="D41" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -4644,13 +4695,13 @@
   <sheetData>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="2:7">
@@ -4658,20 +4709,20 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4679,167 +4730,167 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="3:11">
       <c r="C45" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I45" s="7"/>
       <c r="K45" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="3:9">
       <c r="C46" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="9:12">
       <c r="I47" s="7"/>
       <c r="L47" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="2:9">
       <c r="B48" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="3:9">
       <c r="C49" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I49" s="7"/>
     </row>
     <row r="52" ht="15.75" spans="3:9">
       <c r="C52" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I52" s="7"/>
     </row>
     <row r="53" ht="15.75" spans="3:9">
       <c r="C53" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I53" s="7"/>
     </row>
     <row r="54" ht="15.75" spans="3:9">
       <c r="C54" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I54" s="7"/>
     </row>
     <row r="55" ht="15.75" spans="3:9">
       <c r="C55" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I55" s="7"/>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="3:3">
       <c r="C59" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" spans="3:9">
       <c r="C70" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I70" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="3:9">
       <c r="C71" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I71" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4862,107 +4913,107 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4985,62 +5036,62 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primer informe con filtro like para ireport de productos
SELECT * FROM TIENDA.PRODUCTO where TIENDA.PRODUCTO.descripcion LIKE $P{filtro}
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23955" windowHeight="9735" tabRatio="916" activeTab="1"/>
+    <workbookView windowWidth="23895" windowHeight="9555" tabRatio="916" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="NECESIDADES" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="enlaces y recursos JAVA" sheetId="4" r:id="rId5"/>
     <sheet name="LIBRERIAS Y POM ORG PROY" sheetId="6" r:id="rId6"/>
     <sheet name="ICONOS" sheetId="7" r:id="rId7"/>
+    <sheet name="java se" sheetId="8" r:id="rId8"/>
+    <sheet name="IREPORT PARAMETROS" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="348">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -1081,20 +1083,63 @@
   <si>
     <t>https://www.mingcute.com/</t>
   </si>
+  <si>
+    <t>Descargar Java para Windows</t>
+  </si>
+  <si>
+    <t>https://www.java.com/es/download/ie_manual.jsp</t>
+  </si>
+  <si>
+    <t>Parametros en informes ireports</t>
+  </si>
+  <si>
+    <t>pagina web:</t>
+  </si>
+  <si>
+    <t>https://www.javatutoriales.com/2009/03/creacion-de-reportes-con-jasperrepots-y_30.html</t>
+  </si>
+  <si>
+    <t>videro</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qmWVqZ1UvOE</t>
+  </si>
+  <si>
+    <t>SELECT * FROM TIENDA.PRODUCTO where TIENDA.PRODUCTO.descripcion like $P{filtro}</t>
+  </si>
+  <si>
+    <t>EJEMPLOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://java.hotexamples.com/es/examples/net.sf.jasperreports.engine/JasperFillManager/fillReport/java-jasperfillmanager-fillreport-method-examples.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="34">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF111111"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -1153,14 +1198,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -1174,30 +1211,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1212,6 +1226,43 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1227,18 +1278,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1264,45 +1345,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1376,13 +1421,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1394,7 +1451,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1406,7 +1475,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1418,133 +1583,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1604,15 +1649,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -1630,6 +1666,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1683,221 +1743,210 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1910,10 +1959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1922,16 +1968,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2494,7 +2540,7 @@
   <sheetFormatPr defaultColWidth="11.552380952381" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -2593,7 +2639,7 @@
   <sheetPr/>
   <dimension ref="C2:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A4" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -2611,20 +2657,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="3:11">
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="K3" t="s">
         <v>20</v>
       </c>
@@ -2640,74 +2686,74 @@
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="41" t="s">
         <v>30</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" ht="21" spans="3:9">
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="31" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="4:9">
-      <c r="D9" s="30">
+      <c r="D9" s="32">
         <v>45</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="32">
         <v>150</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2723,24 +2769,24 @@
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="3:8">
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="33" t="s">
         <v>42</v>
       </c>
       <c r="H14" t="s">
@@ -2748,7 +2794,7 @@
       </c>
     </row>
     <row r="15" spans="3:8">
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="32" t="s">
@@ -2768,49 +2814,49 @@
       </c>
     </row>
     <row r="18" spans="3:3">
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="38" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="3:8">
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="3:9">
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E24" t="s">
@@ -2821,30 +2867,30 @@
       </c>
     </row>
     <row r="25" spans="3:9">
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35" t="s">
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="34"/>
+      <c r="F25" s="35"/>
       <c r="I25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="3:9">
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="38" t="s">
+      <c r="F26" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="39" t="s">
         <v>43</v>
       </c>
       <c r="I26" t="s">
@@ -2852,28 +2898,28 @@
       </c>
     </row>
     <row r="27" ht="21" spans="3:7">
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="39"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" spans="4:6">
-      <c r="D28" s="30">
+      <c r="D28" s="32">
         <v>45</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="32">
         <v>150</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="32" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2912,1636 +2958,1636 @@
   <sheetData>
     <row r="2" ht="13.5"/>
     <row r="3" ht="13.5" spans="2:3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" ht="13.5" spans="2:3">
-      <c r="B4" s="11">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" ht="13.5" spans="2:3">
-      <c r="B5" s="11">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" ht="13.5" spans="2:3">
-      <c r="B6" s="11">
+      <c r="B6" s="13">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" ht="13.5" spans="2:3">
-      <c r="B7" s="11">
+      <c r="B7" s="13">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" ht="13.5" spans="2:3">
-      <c r="B8" s="11">
+      <c r="B8" s="13">
         <v>5</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" ht="13.5" spans="2:3">
-      <c r="B9" s="11">
+      <c r="B9" s="13">
         <v>6</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" ht="13.5" spans="2:3">
-      <c r="B10" s="11">
+      <c r="B10" s="13">
         <v>7</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" ht="13.5" spans="2:3">
-      <c r="B11" s="11">
+      <c r="B11" s="13">
         <v>8</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" ht="13.5" spans="2:3">
-      <c r="B12" s="11">
+      <c r="B12" s="13">
         <v>9</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="13" ht="13.5" spans="2:3">
-      <c r="B13" s="11">
+      <c r="B13" s="13">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" ht="13.5" spans="2:3">
-      <c r="B14" s="11">
+      <c r="B14" s="13">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" ht="13.5" spans="2:3">
-      <c r="B15" s="11">
+      <c r="B15" s="13">
         <v>12</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" ht="13.5" spans="2:3">
-      <c r="B16" s="11">
+      <c r="B16" s="13">
         <v>13</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" ht="13.5" spans="2:3">
-      <c r="B17" s="11">
+      <c r="B17" s="13">
         <v>14</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" ht="13.5" spans="2:3">
-      <c r="B18" s="11">
+      <c r="B18" s="13">
         <v>15</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" ht="13.5" spans="2:3">
-      <c r="B19" s="11">
+      <c r="B19" s="13">
         <v>16</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" ht="13.5" spans="2:3">
-      <c r="B20" s="11">
+      <c r="B20" s="13">
         <v>17</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" ht="13.5" spans="2:3">
-      <c r="B21" s="11">
+      <c r="B21" s="13">
         <v>18</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" ht="13.5" spans="2:3">
-      <c r="B22" s="11">
+      <c r="B22" s="13">
         <v>19</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" ht="13.5" spans="2:3">
-      <c r="B23" s="11">
+      <c r="B23" s="13">
         <v>20</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" ht="13.5" spans="2:3">
-      <c r="B24" s="11">
+      <c r="B24" s="13">
         <v>21</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="25" ht="13.5" spans="2:3">
-      <c r="B25" s="11">
+      <c r="B25" s="13">
         <v>22</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="14" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" ht="13.5" spans="2:3">
-      <c r="B26" s="11">
+      <c r="B26" s="13">
         <v>23</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" ht="13.5" spans="2:3">
-      <c r="B27" s="11">
+      <c r="B27" s="13">
         <v>24</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" ht="13.5" spans="2:3">
-      <c r="B28" s="11">
+      <c r="B28" s="13">
         <v>25</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" ht="13.5" spans="2:3">
-      <c r="B29" s="11">
+      <c r="B29" s="13">
         <v>26</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="30" ht="13.5" spans="2:3">
-      <c r="B30" s="11">
+      <c r="B30" s="13">
         <v>27</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="31" ht="13.5" spans="2:3">
-      <c r="B31" s="11">
+      <c r="B31" s="13">
         <v>28</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" ht="13.5" spans="2:3">
-      <c r="B32" s="11">
+      <c r="B32" s="13">
         <v>29</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" ht="13.5" spans="2:3">
-      <c r="B33" s="11">
+      <c r="B33" s="13">
         <v>30</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" ht="13.5" spans="2:3">
-      <c r="B34" s="11">
+      <c r="B34" s="13">
         <v>31</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" ht="13.5" spans="2:3">
-      <c r="B35" s="11">
+      <c r="B35" s="13">
         <v>32</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="36" ht="13.5" spans="2:3">
-      <c r="B36" s="11">
+      <c r="B36" s="13">
         <v>33</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" ht="13.5" spans="2:3">
-      <c r="B37" s="11">
+      <c r="B37" s="13">
         <v>34</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="38" ht="13.5" spans="2:3">
-      <c r="B38" s="11">
+      <c r="B38" s="13">
         <v>35</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="15" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="39" ht="13.5" spans="2:3">
-      <c r="B39" s="11">
+      <c r="B39" s="13">
         <v>36</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="40" ht="13.5" spans="2:3">
-      <c r="B40" s="11">
+      <c r="B40" s="13">
         <v>37</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="41" ht="13.5" spans="2:3">
-      <c r="B41" s="11">
+      <c r="B41" s="13">
         <v>38</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="42" ht="13.5" spans="2:3">
-      <c r="B42" s="11">
+      <c r="B42" s="13">
         <v>39</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="43" ht="13.5" spans="2:3">
-      <c r="B43" s="11">
+      <c r="B43" s="13">
         <v>40</v>
       </c>
-      <c r="C43" s="14"/>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" ht="13.5" spans="2:3">
-      <c r="B44" s="11">
+      <c r="B44" s="13">
         <v>41</v>
       </c>
-      <c r="C44" s="14"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" ht="13.5" spans="2:3">
-      <c r="B45" s="11">
+      <c r="B45" s="13">
         <v>42</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="46" ht="13.5" spans="2:3">
-      <c r="B46" s="11">
+      <c r="B46" s="13">
         <v>43</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="47" ht="13.5" spans="2:3">
-      <c r="B47" s="11">
+      <c r="B47" s="13">
         <v>44</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="48" ht="13.5" spans="2:3">
-      <c r="B48" s="11">
+      <c r="B48" s="13">
         <v>45</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="49" ht="13.5" spans="2:3">
-      <c r="B49" s="11">
+      <c r="B49" s="13">
         <v>46</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="50" ht="13.5" spans="2:3">
-      <c r="B50" s="11">
+      <c r="B50" s="13">
         <v>47</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="51" ht="13.5" spans="2:3">
-      <c r="B51" s="11">
+      <c r="B51" s="13">
         <v>48</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="14" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="52" ht="13.5" spans="2:3">
-      <c r="B52" s="11">
+      <c r="B52" s="13">
         <v>49</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="14" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="53" ht="13.5" spans="2:3">
-      <c r="B53" s="11">
+      <c r="B53" s="13">
         <v>50</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="54" ht="13.5" spans="2:3">
-      <c r="B54" s="11">
+      <c r="B54" s="13">
         <v>51</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="55" ht="13.5" spans="2:3">
-      <c r="B55" s="11">
+      <c r="B55" s="13">
         <v>52</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56" ht="13.5" spans="2:3">
-      <c r="B56" s="11">
+      <c r="B56" s="13">
         <v>53</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="18" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="57" ht="13.5" spans="2:3">
-      <c r="B57" s="11">
+      <c r="B57" s="13">
         <v>54</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="18" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="58" ht="13.5" spans="2:3">
-      <c r="B58" s="11">
+      <c r="B58" s="13">
         <v>55</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="18" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="59" ht="13.5" spans="2:3">
-      <c r="B59" s="11">
+      <c r="B59" s="13">
         <v>56</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="18" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="60" ht="13.5" spans="2:3">
-      <c r="B60" s="11">
+      <c r="B60" s="13">
         <v>57</v>
       </c>
-      <c r="C60" s="17"/>
+      <c r="C60" s="19"/>
     </row>
     <row r="61" ht="13.5" spans="2:3">
-      <c r="B61" s="11">
+      <c r="B61" s="13">
         <v>58</v>
       </c>
-      <c r="C61" s="18"/>
+      <c r="C61" s="20"/>
     </row>
     <row r="62" ht="13.5" spans="2:3">
-      <c r="B62" s="11">
+      <c r="B62" s="13">
         <v>59</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="21" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="63" ht="13.5" spans="2:3">
-      <c r="B63" s="11">
+      <c r="B63" s="13">
         <v>60</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="22" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="64" ht="13.5" spans="2:3">
-      <c r="B64" s="11">
+      <c r="B64" s="13">
         <v>61</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="22" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="65" ht="13.5" spans="2:3">
-      <c r="B65" s="11">
+      <c r="B65" s="13">
         <v>62</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="22" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="66" ht="13.5" spans="2:3">
-      <c r="B66" s="11">
+      <c r="B66" s="13">
         <v>63</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="22" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="67" ht="13.5" spans="2:3">
-      <c r="B67" s="11">
+      <c r="B67" s="13">
         <v>64</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="22" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="68" ht="13.5" spans="2:3">
-      <c r="B68" s="11">
+      <c r="B68" s="13">
         <v>65</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="22" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="69" ht="13.5" spans="2:3">
-      <c r="B69" s="11">
+      <c r="B69" s="13">
         <v>66</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="22" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="2:3">
-      <c r="B70" s="11">
+      <c r="B70" s="13">
         <v>67</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="22" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="2:3">
-      <c r="B71" s="11">
+      <c r="B71" s="13">
         <v>68</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="22" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="2:3">
-      <c r="B72" s="11">
+      <c r="B72" s="13">
         <v>69</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="22" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="2:3">
-      <c r="B73" s="11">
+      <c r="B73" s="13">
         <v>70</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="22" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="74" ht="13.5" spans="2:3">
-      <c r="B74" s="11">
+      <c r="B74" s="13">
         <v>71</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="22" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="75" ht="13.5" spans="2:3">
-      <c r="B75" s="11">
+      <c r="B75" s="13">
         <v>72</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="22" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="76" ht="13.5" spans="2:3">
-      <c r="B76" s="11">
+      <c r="B76" s="13">
         <v>73</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="22" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="77" ht="13.5" spans="2:3">
-      <c r="B77" s="11">
+      <c r="B77" s="13">
         <v>74</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="22" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="78" ht="13.5" spans="2:3">
-      <c r="B78" s="11">
+      <c r="B78" s="13">
         <v>75</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="22" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="79" ht="13.5" spans="2:3">
-      <c r="B79" s="11">
+      <c r="B79" s="13">
         <v>76</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="22" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="80" ht="13.5" spans="2:3">
-      <c r="B80" s="11">
+      <c r="B80" s="13">
         <v>77</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C80" s="22" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="81" ht="13.5" spans="2:3">
-      <c r="B81" s="11">
+      <c r="B81" s="13">
         <v>78</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="C81" s="22" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="82" ht="13.5" spans="2:3">
-      <c r="B82" s="11">
+      <c r="B82" s="13">
         <v>79</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="22" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="83" ht="13.5" spans="2:3">
-      <c r="B83" s="11">
+      <c r="B83" s="13">
         <v>80</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="C83" s="22" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="84" ht="13.5" spans="2:3">
-      <c r="B84" s="11">
+      <c r="B84" s="13">
         <v>81</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="22" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="85" ht="13.5" spans="2:3">
-      <c r="B85" s="11">
+      <c r="B85" s="13">
         <v>82</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C85" s="22" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="86" ht="13.5" spans="2:3">
-      <c r="B86" s="11">
+      <c r="B86" s="13">
         <v>83</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C86" s="22" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="87" ht="13.5" spans="2:3">
-      <c r="B87" s="11">
+      <c r="B87" s="13">
         <v>84</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="22" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="88" ht="13.5" spans="2:3">
-      <c r="B88" s="11">
+      <c r="B88" s="13">
         <v>85</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C88" s="22" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="89" ht="13.5" spans="2:3">
-      <c r="B89" s="11">
+      <c r="B89" s="13">
         <v>86</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C89" s="22" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="90" ht="13.5" spans="2:3">
-      <c r="B90" s="11">
+      <c r="B90" s="13">
         <v>87</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="22" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="2:3">
-      <c r="B91" s="11">
+      <c r="B91" s="13">
         <v>88</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="22" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="2:3">
-      <c r="B92" s="11">
+      <c r="B92" s="13">
         <v>89</v>
       </c>
-      <c r="C92" s="20" t="s">
+      <c r="C92" s="22" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="2:3">
-      <c r="B93" s="11">
+      <c r="B93" s="13">
         <v>90</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="22" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="2:3">
-      <c r="B94" s="11">
+      <c r="B94" s="13">
         <v>91</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="22" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="95" ht="13.5" spans="2:3">
-      <c r="B95" s="11">
+      <c r="B95" s="13">
         <v>92</v>
       </c>
-      <c r="C95" s="20" t="s">
+      <c r="C95" s="22" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="96" ht="13.5" spans="2:3">
-      <c r="B96" s="11">
+      <c r="B96" s="13">
         <v>93</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="C96" s="22" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="97" ht="13.5" spans="2:3">
-      <c r="B97" s="11">
+      <c r="B97" s="13">
         <v>94</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="22" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="98" ht="13.5" spans="2:3">
-      <c r="B98" s="11">
+      <c r="B98" s="13">
         <v>95</v>
       </c>
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="22" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="99" ht="13.5" spans="2:3">
-      <c r="B99" s="11">
+      <c r="B99" s="13">
         <v>96</v>
       </c>
-      <c r="C99" s="20" t="s">
+      <c r="C99" s="22" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="100" ht="13.5" spans="2:3">
-      <c r="B100" s="11">
+      <c r="B100" s="13">
         <v>97</v>
       </c>
-      <c r="C100" s="20" t="s">
+      <c r="C100" s="22" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="101" ht="13.5" spans="2:3">
-      <c r="B101" s="11">
+      <c r="B101" s="13">
         <v>98</v>
       </c>
-      <c r="C101" s="14"/>
+      <c r="C101" s="16"/>
     </row>
     <row r="102" ht="13.5" spans="2:3">
-      <c r="B102" s="11">
+      <c r="B102" s="13">
         <v>99</v>
       </c>
-      <c r="C102" s="14"/>
+      <c r="C102" s="16"/>
     </row>
     <row r="103" ht="13.5" spans="2:3">
-      <c r="B103" s="11">
+      <c r="B103" s="13">
         <v>100</v>
       </c>
-      <c r="C103" s="15" t="s">
+      <c r="C103" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="104" ht="13.5" spans="2:3">
-      <c r="B104" s="11">
+      <c r="B104" s="13">
         <v>101</v>
       </c>
-      <c r="C104" s="12" t="s">
+      <c r="C104" s="14" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="105" ht="13.5" spans="2:3">
-      <c r="B105" s="11">
+      <c r="B105" s="13">
         <v>102</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="15" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="106" ht="13.5" spans="2:3">
-      <c r="B106" s="11">
+      <c r="B106" s="13">
         <v>103</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="15" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="107" ht="13.5" spans="2:3">
-      <c r="B107" s="11">
+      <c r="B107" s="13">
         <v>104</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C107" s="15" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="108" ht="13.5" spans="2:3">
-      <c r="B108" s="11">
+      <c r="B108" s="13">
         <v>105</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C108" s="15" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="109" ht="13.5" spans="2:3">
-      <c r="B109" s="11">
+      <c r="B109" s="13">
         <v>106</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="15" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="110" ht="13.5" spans="2:3">
-      <c r="B110" s="11">
+      <c r="B110" s="13">
         <v>107</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C110" s="15" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="111" ht="13.5" spans="2:3">
-      <c r="B111" s="11">
+      <c r="B111" s="13">
         <v>108</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="15" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="112" ht="13.5" spans="2:3">
-      <c r="B112" s="11">
+      <c r="B112" s="13">
         <v>109</v>
       </c>
-      <c r="C112" s="13" t="s">
+      <c r="C112" s="15" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="113" ht="13.5" spans="2:3">
-      <c r="B113" s="11">
+      <c r="B113" s="13">
         <v>110</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="15" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="114" ht="13.5" spans="2:3">
-      <c r="B114" s="11">
+      <c r="B114" s="13">
         <v>111</v>
       </c>
-      <c r="C114" s="13" t="s">
+      <c r="C114" s="15" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="115" ht="13.5" spans="2:3">
-      <c r="B115" s="11">
+      <c r="B115" s="13">
         <v>112</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C115" s="15" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="116" ht="13.5" spans="2:3">
-      <c r="B116" s="11">
+      <c r="B116" s="13">
         <v>113</v>
       </c>
-      <c r="C116" s="13" t="s">
+      <c r="C116" s="15" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="117" ht="13.5" spans="2:3">
-      <c r="B117" s="11">
+      <c r="B117" s="13">
         <v>114</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="C117" s="15" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="118" ht="13.5" spans="2:3">
-      <c r="B118" s="11">
+      <c r="B118" s="13">
         <v>115</v>
       </c>
-      <c r="C118" s="21" t="s">
+      <c r="C118" s="23" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="119" ht="13.5" spans="2:3">
-      <c r="B119" s="11">
+      <c r="B119" s="13">
         <v>116</v>
       </c>
-      <c r="C119" s="21" t="s">
+      <c r="C119" s="23" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="120" ht="13.5" spans="2:3">
-      <c r="B120" s="11">
+      <c r="B120" s="13">
         <v>117</v>
       </c>
-      <c r="C120" s="21" t="s">
+      <c r="C120" s="23" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="121" ht="13.5" spans="2:3">
-      <c r="B121" s="11">
+      <c r="B121" s="13">
         <v>118</v>
       </c>
-      <c r="C121" s="21" t="s">
+      <c r="C121" s="23" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="122" ht="13.5" spans="2:3">
-      <c r="B122" s="11">
+      <c r="B122" s="13">
         <v>119</v>
       </c>
-      <c r="C122" s="21" t="s">
+      <c r="C122" s="23" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="123" ht="13.5" spans="2:3">
-      <c r="B123" s="11">
+      <c r="B123" s="13">
         <v>120</v>
       </c>
-      <c r="C123" s="21" t="s">
+      <c r="C123" s="23" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="124" ht="13.5" spans="2:3">
-      <c r="B124" s="11">
+      <c r="B124" s="13">
         <v>121</v>
       </c>
-      <c r="C124" s="21" t="s">
+      <c r="C124" s="23" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="125" ht="13.5" spans="2:3">
-      <c r="B125" s="11">
+      <c r="B125" s="13">
         <v>122</v>
       </c>
-      <c r="C125" s="21" t="s">
+      <c r="C125" s="23" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="126" ht="13.5" spans="2:3">
-      <c r="B126" s="11">
+      <c r="B126" s="13">
         <v>123</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="C126" s="23" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="127" ht="13.5" spans="2:3">
-      <c r="B127" s="11">
+      <c r="B127" s="13">
         <v>124</v>
       </c>
-      <c r="C127" s="21" t="s">
+      <c r="C127" s="23" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="128" ht="13.5" spans="2:3">
-      <c r="B128" s="11">
+      <c r="B128" s="13">
         <v>125</v>
       </c>
-      <c r="C128" s="21" t="s">
+      <c r="C128" s="23" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="129" ht="13.5" spans="2:3">
-      <c r="B129" s="11">
+      <c r="B129" s="13">
         <v>126</v>
       </c>
-      <c r="C129" s="21" t="s">
+      <c r="C129" s="23" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="130" ht="13.5" spans="2:3">
-      <c r="B130" s="11">
+      <c r="B130" s="13">
         <v>127</v>
       </c>
-      <c r="C130" s="21" t="s">
+      <c r="C130" s="23" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="131" ht="13.5" spans="2:3">
-      <c r="B131" s="11">
+      <c r="B131" s="13">
         <v>128</v>
       </c>
-      <c r="C131" s="21" t="s">
+      <c r="C131" s="23" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="132" ht="13.5" spans="2:3">
-      <c r="B132" s="11">
+      <c r="B132" s="13">
         <v>129</v>
       </c>
-      <c r="C132" s="12" t="s">
+      <c r="C132" s="14" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="133" ht="13.5" spans="2:3">
-      <c r="B133" s="11">
+      <c r="B133" s="13">
         <v>130</v>
       </c>
-      <c r="C133" s="12" t="s">
+      <c r="C133" s="14" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="134" ht="13.5" spans="2:3">
-      <c r="B134" s="11">
+      <c r="B134" s="13">
         <v>131</v>
       </c>
-      <c r="C134" s="12" t="s">
+      <c r="C134" s="14" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="135" ht="13.5" spans="2:3">
-      <c r="B135" s="11">
+      <c r="B135" s="13">
         <v>132</v>
       </c>
-      <c r="C135" s="12" t="s">
+      <c r="C135" s="14" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="136" ht="13.5" spans="2:3">
-      <c r="B136" s="11">
+      <c r="B136" s="13">
         <v>133</v>
       </c>
-      <c r="C136" s="12" t="s">
+      <c r="C136" s="14" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="137" ht="13.5" spans="2:3">
-      <c r="B137" s="11">
+      <c r="B137" s="13">
         <v>134</v>
       </c>
-      <c r="C137" s="16" t="s">
+      <c r="C137" s="18" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="138" ht="13.5" spans="2:3">
-      <c r="B138" s="11">
+      <c r="B138" s="13">
         <v>135</v>
       </c>
-      <c r="C138" s="16" t="s">
+      <c r="C138" s="18" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="139" ht="13.5" spans="2:3">
-      <c r="B139" s="11">
+      <c r="B139" s="13">
         <v>136</v>
       </c>
-      <c r="C139" s="16" t="s">
+      <c r="C139" s="18" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="140" ht="13.5" spans="2:3">
-      <c r="B140" s="11">
+      <c r="B140" s="13">
         <v>137</v>
       </c>
-      <c r="C140" s="22" t="s">
+      <c r="C140" s="24" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="141" ht="13.5" spans="2:3">
-      <c r="B141" s="11">
+      <c r="B141" s="13">
         <v>138</v>
       </c>
-      <c r="C141" s="22" t="s">
+      <c r="C141" s="24" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="142" ht="13.5" spans="2:3">
-      <c r="B142" s="11">
+      <c r="B142" s="13">
         <v>139</v>
       </c>
-      <c r="C142" s="22" t="s">
+      <c r="C142" s="24" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="143" ht="13.5" spans="2:3">
-      <c r="B143" s="11">
+      <c r="B143" s="13">
         <v>140</v>
       </c>
-      <c r="C143" s="22" t="s">
+      <c r="C143" s="24" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="144" ht="13.5" spans="2:3">
-      <c r="B144" s="11">
+      <c r="B144" s="13">
         <v>141</v>
       </c>
-      <c r="C144" s="22" t="s">
+      <c r="C144" s="24" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="145" ht="13.5" spans="2:3">
-      <c r="B145" s="11">
+      <c r="B145" s="13">
         <v>142</v>
       </c>
-      <c r="C145" s="22" t="s">
+      <c r="C145" s="24" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="146" ht="13.5" spans="2:3">
-      <c r="B146" s="11">
+      <c r="B146" s="13">
         <v>143</v>
       </c>
-      <c r="C146" s="22" t="s">
+      <c r="C146" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="147" ht="13.5" spans="2:3">
-      <c r="B147" s="11">
+      <c r="B147" s="13">
         <v>144</v>
       </c>
-      <c r="C147" s="22" t="s">
+      <c r="C147" s="24" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="148" ht="13.5" spans="2:3">
-      <c r="B148" s="11">
+      <c r="B148" s="13">
         <v>145</v>
       </c>
-      <c r="C148" s="22" t="s">
+      <c r="C148" s="24" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="149" ht="13.5" spans="2:3">
-      <c r="B149" s="11">
+      <c r="B149" s="13">
         <v>146</v>
       </c>
-      <c r="C149" s="23" t="s">
+      <c r="C149" s="25" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="150" ht="13.5" spans="2:3">
-      <c r="B150" s="11">
+      <c r="B150" s="13">
         <v>147</v>
       </c>
-      <c r="C150" s="13" t="s">
+      <c r="C150" s="15" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="151" ht="13.5" spans="2:3">
-      <c r="B151" s="11">
+      <c r="B151" s="13">
         <v>148</v>
       </c>
-      <c r="C151" s="13" t="s">
+      <c r="C151" s="15" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="152" ht="13.5" spans="2:3">
-      <c r="B152" s="11">
+      <c r="B152" s="13">
         <v>149</v>
       </c>
-      <c r="C152" s="13" t="s">
+      <c r="C152" s="15" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="153" ht="13.5" spans="2:3">
-      <c r="B153" s="11">
+      <c r="B153" s="13">
         <v>150</v>
       </c>
-      <c r="C153" s="14"/>
+      <c r="C153" s="16"/>
     </row>
     <row r="154" ht="13.5" spans="2:3">
-      <c r="B154" s="11">
+      <c r="B154" s="13">
         <v>151</v>
       </c>
-      <c r="C154" s="14"/>
+      <c r="C154" s="16"/>
     </row>
     <row r="155" ht="13.5" spans="2:3">
-      <c r="B155" s="11">
+      <c r="B155" s="13">
         <v>152</v>
       </c>
-      <c r="C155" s="24" t="s">
+      <c r="C155" s="26" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="156" ht="13.5" spans="2:3">
-      <c r="B156" s="11">
+      <c r="B156" s="13">
         <v>153</v>
       </c>
-      <c r="C156" s="23" t="s">
+      <c r="C156" s="25" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="157" ht="13.5" spans="2:3">
-      <c r="B157" s="11">
+      <c r="B157" s="13">
         <v>154</v>
       </c>
-      <c r="C157" s="23" t="s">
+      <c r="C157" s="25" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="158" ht="13.5" spans="2:3">
-      <c r="B158" s="11">
+      <c r="B158" s="13">
         <v>155</v>
       </c>
-      <c r="C158" s="23" t="s">
+      <c r="C158" s="25" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="159" ht="13.5" spans="2:3">
-      <c r="B159" s="11">
+      <c r="B159" s="13">
         <v>156</v>
       </c>
-      <c r="C159" s="23" t="s">
+      <c r="C159" s="25" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="160" ht="13.5" spans="2:3">
-      <c r="B160" s="11">
+      <c r="B160" s="13">
         <v>157</v>
       </c>
-      <c r="C160" s="23" t="s">
+      <c r="C160" s="25" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="161" ht="13.5" spans="2:3">
-      <c r="B161" s="11">
+      <c r="B161" s="13">
         <v>158</v>
       </c>
-      <c r="C161" s="23" t="s">
+      <c r="C161" s="25" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="162" ht="13.5" spans="2:3">
-      <c r="B162" s="11">
+      <c r="B162" s="13">
         <v>159</v>
       </c>
-      <c r="C162" s="23" t="s">
+      <c r="C162" s="25" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="163" ht="13.5" spans="2:3">
-      <c r="B163" s="11">
+      <c r="B163" s="13">
         <v>160</v>
       </c>
-      <c r="C163" s="23" t="s">
+      <c r="C163" s="25" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="164" ht="13.5" spans="2:3">
-      <c r="B164" s="11">
+      <c r="B164" s="13">
         <v>161</v>
       </c>
-      <c r="C164" s="23" t="s">
+      <c r="C164" s="25" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="165" ht="13.5" spans="2:3">
-      <c r="B165" s="11">
+      <c r="B165" s="13">
         <v>162</v>
       </c>
-      <c r="C165" s="23" t="s">
+      <c r="C165" s="25" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="166" ht="13.5" spans="2:3">
-      <c r="B166" s="11">
+      <c r="B166" s="13">
         <v>163</v>
       </c>
-      <c r="C166" s="23" t="s">
+      <c r="C166" s="25" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="167" ht="13.5" spans="2:3">
-      <c r="B167" s="11">
+      <c r="B167" s="13">
         <v>164</v>
       </c>
-      <c r="C167" s="23" t="s">
+      <c r="C167" s="25" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="168" ht="13.5" spans="2:3">
-      <c r="B168" s="11">
+      <c r="B168" s="13">
         <v>165</v>
       </c>
-      <c r="C168" s="23" t="s">
+      <c r="C168" s="25" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="169" ht="13.5" spans="2:3">
-      <c r="B169" s="11">
+      <c r="B169" s="13">
         <v>166</v>
       </c>
-      <c r="C169" s="14"/>
+      <c r="C169" s="16"/>
     </row>
     <row r="170" ht="13.5" spans="2:3">
-      <c r="B170" s="11">
+      <c r="B170" s="13">
         <v>167</v>
       </c>
-      <c r="C170" s="18"/>
+      <c r="C170" s="20"/>
     </row>
     <row r="171" ht="13.5" spans="2:3">
-      <c r="B171" s="11">
+      <c r="B171" s="13">
         <v>168</v>
       </c>
-      <c r="C171" s="19" t="s">
+      <c r="C171" s="21" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="172" ht="13.5" spans="2:3">
-      <c r="B172" s="11">
+      <c r="B172" s="13">
         <v>169</v>
       </c>
-      <c r="C172" s="12" t="s">
+      <c r="C172" s="14" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="173" ht="13.5" spans="2:3">
-      <c r="B173" s="11">
+      <c r="B173" s="13">
         <v>170</v>
       </c>
-      <c r="C173" s="12" t="s">
+      <c r="C173" s="14" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="174" ht="13.5" spans="2:3">
-      <c r="B174" s="11">
+      <c r="B174" s="13">
         <v>171</v>
       </c>
-      <c r="C174" s="12" t="s">
+      <c r="C174" s="14" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="175" ht="13.5" spans="2:3">
-      <c r="B175" s="11">
+      <c r="B175" s="13">
         <v>172</v>
       </c>
-      <c r="C175" s="12" t="s">
+      <c r="C175" s="14" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="176" ht="13.5" spans="2:3">
-      <c r="B176" s="11">
+      <c r="B176" s="13">
         <v>173</v>
       </c>
-      <c r="C176" s="12" t="s">
+      <c r="C176" s="14" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="177" ht="13.5" spans="2:3">
-      <c r="B177" s="11">
+      <c r="B177" s="13">
         <v>174</v>
       </c>
-      <c r="C177" s="12" t="s">
+      <c r="C177" s="14" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="178" ht="13.5" spans="2:3">
-      <c r="B178" s="11">
+      <c r="B178" s="13">
         <v>175</v>
       </c>
-      <c r="C178" s="12" t="s">
+      <c r="C178" s="14" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="179" ht="13.5" spans="2:3">
-      <c r="B179" s="11">
+      <c r="B179" s="13">
         <v>176</v>
       </c>
-      <c r="C179" s="12" t="s">
+      <c r="C179" s="14" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="180" ht="13.5" spans="2:3">
-      <c r="B180" s="11">
+      <c r="B180" s="13">
         <v>177</v>
       </c>
-      <c r="C180" s="12" t="s">
+      <c r="C180" s="14" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="181" ht="13.5" spans="2:3">
-      <c r="B181" s="11">
+      <c r="B181" s="13">
         <v>178</v>
       </c>
-      <c r="C181" s="12" t="s">
+      <c r="C181" s="14" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="182" ht="13.5" spans="2:3">
-      <c r="B182" s="11">
+      <c r="B182" s="13">
         <v>179</v>
       </c>
-      <c r="C182" s="12" t="s">
+      <c r="C182" s="14" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="183" ht="13.5" spans="2:3">
-      <c r="B183" s="11">
+      <c r="B183" s="13">
         <v>180</v>
       </c>
-      <c r="C183" s="12" t="s">
+      <c r="C183" s="14" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="184" ht="13.5" spans="2:3">
-      <c r="B184" s="11">
+      <c r="B184" s="13">
         <v>181</v>
       </c>
-      <c r="C184" s="12" t="s">
+      <c r="C184" s="14" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="185" ht="13.5" spans="2:3">
-      <c r="B185" s="11">
+      <c r="B185" s="13">
         <v>182</v>
       </c>
-      <c r="C185" s="12" t="s">
+      <c r="C185" s="14" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="186" ht="13.5" spans="2:3">
-      <c r="B186" s="11">
+      <c r="B186" s="13">
         <v>183</v>
       </c>
-      <c r="C186" s="12" t="s">
+      <c r="C186" s="14" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="187" ht="13.5" spans="2:3">
-      <c r="B187" s="11">
+      <c r="B187" s="13">
         <v>184</v>
       </c>
-      <c r="C187" s="12" t="s">
+      <c r="C187" s="14" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="188" ht="13.5" spans="2:3">
-      <c r="B188" s="11">
+      <c r="B188" s="13">
         <v>185</v>
       </c>
-      <c r="C188" s="14"/>
+      <c r="C188" s="16"/>
     </row>
     <row r="189" ht="13.5" spans="2:3">
-      <c r="B189" s="11">
+      <c r="B189" s="13">
         <v>186</v>
       </c>
-      <c r="C189" s="14"/>
+      <c r="C189" s="16"/>
     </row>
     <row r="190" ht="13.5" spans="2:3">
-      <c r="B190" s="11">
+      <c r="B190" s="13">
         <v>187</v>
       </c>
-      <c r="C190" s="19" t="s">
+      <c r="C190" s="21" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="191" ht="13.5" spans="2:3">
-      <c r="B191" s="11">
+      <c r="B191" s="13">
         <v>188</v>
       </c>
-      <c r="C191" s="12" t="s">
+      <c r="C191" s="14" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="192" ht="13.5" spans="2:3">
-      <c r="B192" s="11">
+      <c r="B192" s="13">
         <v>189</v>
       </c>
-      <c r="C192" s="12" t="s">
+      <c r="C192" s="14" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="193" ht="13.5" spans="2:3">
-      <c r="B193" s="11">
+      <c r="B193" s="13">
         <v>190</v>
       </c>
-      <c r="C193" s="12" t="s">
+      <c r="C193" s="14" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="194" ht="13.5" spans="2:3">
-      <c r="B194" s="11">
+      <c r="B194" s="13">
         <v>191</v>
       </c>
-      <c r="C194" s="12" t="s">
+      <c r="C194" s="14" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="195" ht="13.5" spans="2:3">
-      <c r="B195" s="11">
+      <c r="B195" s="13">
         <v>192</v>
       </c>
-      <c r="C195" s="12" t="s">
+      <c r="C195" s="14" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="196" ht="13.5" spans="2:3">
-      <c r="B196" s="11">
+      <c r="B196" s="13">
         <v>193</v>
       </c>
-      <c r="C196" s="12" t="s">
+      <c r="C196" s="14" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="197" ht="13.5" spans="2:3">
-      <c r="B197" s="11">
+      <c r="B197" s="13">
         <v>194</v>
       </c>
-      <c r="C197" s="12" t="s">
+      <c r="C197" s="14" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="198" ht="13.5" spans="2:3">
-      <c r="B198" s="11">
+      <c r="B198" s="13">
         <v>195</v>
       </c>
-      <c r="C198" s="12" t="s">
+      <c r="C198" s="14" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="199" ht="13.5" spans="2:3">
-      <c r="B199" s="11">
+      <c r="B199" s="13">
         <v>196</v>
       </c>
-      <c r="C199" s="18"/>
+      <c r="C199" s="20"/>
     </row>
     <row r="200" ht="13.5" spans="2:3">
-      <c r="B200" s="11">
+      <c r="B200" s="13">
         <v>197</v>
       </c>
-      <c r="C200" s="18"/>
+      <c r="C200" s="20"/>
     </row>
     <row r="201" ht="13.5" spans="2:3">
-      <c r="B201" s="11">
+      <c r="B201" s="13">
         <v>198</v>
       </c>
-      <c r="C201" s="19" t="s">
+      <c r="C201" s="21" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="202" ht="13.5" spans="2:3">
-      <c r="B202" s="11">
+      <c r="B202" s="13">
         <v>199</v>
       </c>
-      <c r="C202" s="12" t="s">
+      <c r="C202" s="14" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="203" ht="13.5" spans="2:3">
-      <c r="B203" s="11">
+      <c r="B203" s="13">
         <v>200</v>
       </c>
-      <c r="C203" s="12" t="s">
+      <c r="C203" s="14" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="204" ht="13.5" spans="2:3">
-      <c r="B204" s="11">
+      <c r="B204" s="13">
         <v>201</v>
       </c>
-      <c r="C204" s="12" t="s">
+      <c r="C204" s="14" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="205" ht="13.5" spans="2:3">
-      <c r="B205" s="11">
+      <c r="B205" s="13">
         <v>202</v>
       </c>
-      <c r="C205" s="12" t="s">
+      <c r="C205" s="14" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="206" ht="13.5" spans="2:3">
-      <c r="B206" s="11">
+      <c r="B206" s="13">
         <v>203</v>
       </c>
-      <c r="C206" s="12" t="s">
+      <c r="C206" s="14" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="207" ht="13.5" spans="2:3">
-      <c r="B207" s="11">
+      <c r="B207" s="13">
         <v>204</v>
       </c>
-      <c r="C207" s="12" t="s">
+      <c r="C207" s="14" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="208" ht="13.5" spans="2:3">
-      <c r="B208" s="11">
+      <c r="B208" s="13">
         <v>205</v>
       </c>
-      <c r="C208" s="12" t="s">
+      <c r="C208" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="209" ht="13.5" spans="2:3">
-      <c r="B209" s="11">
+      <c r="B209" s="13">
         <v>206</v>
       </c>
-      <c r="C209" s="18"/>
+      <c r="C209" s="20"/>
     </row>
     <row r="210" ht="13.5" spans="2:3">
-      <c r="B210" s="11">
+      <c r="B210" s="13">
         <v>207</v>
       </c>
-      <c r="C210" s="18"/>
+      <c r="C210" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4561,75 +4607,75 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" ht="27" customHeight="1" spans="1:13">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>249</v>
       </c>
       <c r="F3" t="s">
         <v>250</v>
       </c>
-      <c r="O3" s="9"/>
+      <c r="O3" s="11"/>
       <c r="Q3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="4" spans="15:15">
-      <c r="O4" s="9"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="3:15">
       <c r="C5" t="s">
         <v>252</v>
       </c>
-      <c r="O5" s="9"/>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="15:15">
-      <c r="O6" s="9"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="5:15">
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="O7" s="9"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="6:15">
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="O8" s="9"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="6:15">
       <c r="F9" t="s">
         <v>255</v>
       </c>
-      <c r="O9" s="9"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" spans="6:15">
       <c r="F10" t="s">
         <v>256</v>
       </c>
-      <c r="O10" s="9"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" spans="15:15">
-      <c r="O11" s="9"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="15:15">
-      <c r="O12" s="9"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
@@ -4655,7 +4701,7 @@
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>262</v>
       </c>
     </row>
@@ -4690,14 +4736,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="2"/>
+    <col min="1" max="1" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>266</v>
       </c>
       <c r="I2" t="s">
@@ -4705,7 +4751,7 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G3" t="s">
@@ -4713,10 +4759,10 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4726,7 +4772,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
@@ -4734,7 +4780,7 @@
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4744,7 +4790,7 @@
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>274</v>
       </c>
     </row>
@@ -4754,7 +4800,7 @@
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4764,7 +4810,7 @@
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>278</v>
       </c>
     </row>
@@ -4774,23 +4820,23 @@
       </c>
     </row>
     <row r="45" spans="3:11">
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="I45" s="7"/>
+      <c r="I45" s="9"/>
       <c r="K45" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="46" spans="3:9">
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="I46" s="7"/>
+      <c r="I46" s="9"/>
     </row>
     <row r="47" spans="9:12">
-      <c r="I47" s="7"/>
-      <c r="L47" s="1" t="s">
+      <c r="I47" s="9"/>
+      <c r="L47" s="3" t="s">
         <v>283</v>
       </c>
     </row>
@@ -4798,49 +4844,49 @@
       <c r="B48" t="s">
         <v>284</v>
       </c>
-      <c r="I48" s="7"/>
+      <c r="I48" s="9"/>
     </row>
     <row r="49" spans="3:9">
       <c r="C49" t="s">
         <v>285</v>
       </c>
-      <c r="I49" s="7"/>
+      <c r="I49" s="9"/>
     </row>
     <row r="52" ht="15.75" spans="3:9">
       <c r="C52" t="s">
         <v>286</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="H52" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="I52" s="7"/>
+      <c r="I52" s="9"/>
     </row>
     <row r="53" ht="15.75" spans="3:9">
       <c r="C53" t="s">
         <v>288</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="H53" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="I53" s="7"/>
+      <c r="I53" s="9"/>
     </row>
     <row r="54" ht="15.75" spans="3:9">
       <c r="C54" t="s">
         <v>290</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="H54" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="I54" s="7"/>
+      <c r="I54" s="9"/>
     </row>
     <row r="55" ht="15.75" spans="3:9">
       <c r="C55" t="s">
         <v>292</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H55" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="I55" s="7"/>
+      <c r="I55" s="9"/>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" t="s">
@@ -4868,7 +4914,7 @@
       </c>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="3" t="s">
         <v>299</v>
       </c>
     </row>
@@ -4912,7 +4958,7 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5098,4 +5144,88 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C2:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="2" ht="30" spans="3:3">
+      <c r="C2" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3">
+      <c r="C4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" ht="30" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ejemplo de crear reporte desde jtable
https://www.youtube.com/watch?v=y51JJhZx6FM y ejemplo "Reportes.rar
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="351">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -1113,14 +1113,23 @@
   <si>
     <t xml:space="preserve"> https://java.hotexamples.com/es/examples/net.sf.jasperreports.engine/JasperFillManager/fillReport/java-jasperfillmanager-fillreport-method-examples.html</t>
   </si>
+  <si>
+    <t>Ejemplo de crear reporte (sin usar base de datos, y los datos desdes jtable)</t>
+  </si>
+  <si>
+    <t>Reportes en Java sin Conexion de Base de Datos 2017</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y51JJhZx6FM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1211,7 +1220,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1226,51 +1250,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1278,23 +1257,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1308,6 +1281,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1315,25 +1331,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1345,9 +1354,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1427,43 +1436,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1481,7 +1472,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1493,7 +1502,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1505,91 +1586,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1649,8 +1658,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1670,15 +1712,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1694,17 +1727,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1723,153 +1752,133 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1877,7 +1886,7 @@
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5176,13 +5185,13 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:B19"/>
+  <dimension ref="B1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B22" sqref="B22:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" ht="30" spans="2:2">
       <c r="B1" s="1" t="s">
@@ -5222,6 +5231,21 @@
     <row r="19" spans="2:2">
       <c r="B19" t="s">
         <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
informacion sobre estilos usando POI para excel
Nueva pestaña añadida al  fichero excel "Lineas a Seguir" sobre blog donde explican como añadir y asignar nuevos estilos a celdas excel usando la libreria POI
</commit_message>
<xml_diff>
--- a/Lineas a Seguir.xlsx
+++ b/Lineas a Seguir.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="9555" tabRatio="916" firstSheet="1" activeTab="8"/>
+    <workbookView windowWidth="22890" windowHeight="9555" tabRatio="916" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="NECESIDADES" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="ICONOS" sheetId="7" r:id="rId7"/>
     <sheet name="java se" sheetId="8" r:id="rId8"/>
     <sheet name="IREPORT PARAMETROS" sheetId="9" r:id="rId9"/>
+    <sheet name="POI ESTILOS EN EXCEL" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="357">
   <si>
     <t>NECESITO:</t>
   </si>
@@ -1122,19 +1123,43 @@
   <si>
     <t>https://www.youtube.com/watch?v=y51JJhZx6FM</t>
   </si>
+  <si>
+    <t>Ejemplo de dar formato añadir imagen al reporte</t>
+  </si>
+  <si>
+    <t>Diseñar un Reporte Básico con iReport</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yjqMf6SImRM</t>
+  </si>
+  <si>
+    <t>Apache POI: Cómo definir estilos en archivos excel</t>
+  </si>
+  <si>
+    <t>https://www.pixnbgames.com/blog/excel/apache-poi-como-definir-estilos-en-archivos-excel/</t>
+  </si>
+  <si>
+    <t>https://github.com/angelnavarro/Apache-POI-Examples</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
@@ -1149,12 +1174,6 @@
       <b/>
       <sz val="24"/>
       <color rgb="FF111111"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -1207,18 +1226,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1226,16 +1233,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1250,16 +1261,69 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1287,33 +1351,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1325,30 +1367,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1356,7 +1375,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1430,19 +1449,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1454,31 +1491,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1490,13 +1503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1509,6 +1522,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1532,13 +1569,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,13 +1593,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1568,37 +1617,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1674,6 +1693,51 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1697,36 +1761,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1737,166 +1771,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1955,7 +1974,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1968,7 +1987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2282,6 +2301,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4467225" y="4524375"/>
+          <a:ext cx="5695950" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -2549,7 +2615,7 @@
   <sheetFormatPr defaultColWidth="11.552380952381" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -2640,6 +2706,38 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -4633,7 +4731,7 @@
       <c r="M1" s="10"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>249</v>
       </c>
       <c r="F3" t="s">
@@ -4657,7 +4755,7 @@
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="5:15">
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>253</v>
       </c>
       <c r="O7" s="11"/>
@@ -4710,7 +4808,7 @@
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>262</v>
       </c>
     </row>
@@ -4752,7 +4850,7 @@
       <c r="A2" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>266</v>
       </c>
       <c r="I2" t="s">
@@ -4771,7 +4869,7 @@
       <c r="A5" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4789,7 +4887,7 @@
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4799,7 +4897,7 @@
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>274</v>
       </c>
     </row>
@@ -4809,7 +4907,7 @@
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4819,7 +4917,7 @@
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="1" t="s">
         <v>278</v>
       </c>
     </row>
@@ -4829,7 +4927,7 @@
       </c>
     </row>
     <row r="45" spans="3:11">
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="1" t="s">
         <v>280</v>
       </c>
       <c r="I45" s="9"/>
@@ -4838,14 +4936,14 @@
       </c>
     </row>
     <row r="46" spans="3:9">
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="1" t="s">
         <v>282</v>
       </c>
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="9:12">
       <c r="I47" s="9"/>
-      <c r="L47" s="3" t="s">
+      <c r="L47" s="1" t="s">
         <v>283</v>
       </c>
     </row>
@@ -4923,7 +5021,7 @@
       </c>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="1" t="s">
         <v>299</v>
       </c>
     </row>
@@ -4967,7 +5065,7 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5167,7 +5265,7 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="2"/>
   <sheetData>
     <row r="2" ht="30" spans="3:3">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5185,16 +5283,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:C24"/>
+  <dimension ref="B1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" ht="30" spans="2:2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5248,8 +5346,24 @@
         <v>350</v>
       </c>
     </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>